<commit_message>
Added some more cards
</commit_message>
<xml_diff>
--- a/ShipCardsDesigns.xlsx
+++ b/ShipCardsDesigns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7458491-C5AB-453B-BCBF-5EF588BAEB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BE51CC-67A9-4359-9BCB-215302C573E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{26B571D9-6066-4A50-9F1B-6B43D918E0C1}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="34380" r:id="rId3"/>
+    <pivotCache cacheId="36" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="291">
   <si>
     <t>Type</t>
   </si>
@@ -834,13 +834,164 @@
   </si>
   <si>
     <t>All Robots on target ship get +1 to their department on tap</t>
+  </si>
+  <si>
+    <t>Fighter Bot 2000</t>
+  </si>
+  <si>
+    <t>Can only be tapped to use gun slot.
+When Using gun slot add an aditional 100 damage</t>
+  </si>
+  <si>
+    <t>Attach to crew: This crew member when used on gun slot add aditional 100 damage against a targets ships shield</t>
+  </si>
+  <si>
+    <t>Knowing Shields</t>
+  </si>
+  <si>
+    <t>Attach to crew: This crew member can use one extra gun slot</t>
+  </si>
+  <si>
+    <t>An extra hand</t>
+  </si>
+  <si>
+    <t>Target ship: Switch targets ship shield with its hull</t>
+  </si>
+  <si>
+    <t>Target ship: Restore 200 shield</t>
+  </si>
+  <si>
+    <t>Shield Booster</t>
+  </si>
+  <si>
+    <t>Target ship: Increase shield max by 200 and Restore 200 shield</t>
+  </si>
+  <si>
+    <t>Flick the switch</t>
+  </si>
+  <si>
+    <t>Sometimes you just need to check everythings plugged in.</t>
+  </si>
+  <si>
+    <t>Unidentified Lifeform</t>
+  </si>
+  <si>
+    <t>on Going Event</t>
+  </si>
+  <si>
+    <t>No one has ever known the true purpose of this disgusting lifeform but it just gets in the way</t>
+  </si>
+  <si>
+    <t>Attach to ship: At the start of ship owners turn add a unidentified lifeform token to a empty crew slot. The token cannot be used on gun slots and has: Tap: remove unidentified lifeform and assigned ship takes 100 damage.</t>
+  </si>
+  <si>
+    <t>Evolutionary Pod</t>
+  </si>
+  <si>
+    <t>Attach to ship: All unidentified lifeform tokens can now be used on a gun slot. When a unidentifed lifeform is used on a gun slot it is sacrified and deals an extra 400 to targeted ship</t>
+  </si>
+  <si>
+    <t>Promotion!</t>
+  </si>
+  <si>
+    <t>Tractor Beam</t>
+  </si>
+  <si>
+    <t>Steal target players ship upgrade from target enemy ship and attach to one of your ships</t>
+  </si>
+  <si>
+    <t>Its in the stars</t>
+  </si>
+  <si>
+    <t>Search your strategy deck for any card with converted cost of 4 or less and place into your hand. Then shuffle your strategy deck.</t>
+  </si>
+  <si>
+    <t>Even further beyond</t>
+  </si>
+  <si>
+    <t>Search your strategy deck for any card with converted cost of 4 or less and immediately play without paying its cost. Then shuffle your strategy deck.</t>
+  </si>
+  <si>
+    <t>Fusion Reactor</t>
+  </si>
+  <si>
+    <t>Attach to ship: Increase ships maximum shield by 400 while this is attached. Restore shield back to full when this is first attached.</t>
+  </si>
+  <si>
+    <t>Wires Crossed</t>
+  </si>
+  <si>
+    <t>Search your strategy deck for 1 crew card with a rank higher than 1 and place into your hand. Then shuffle your strategy deck.</t>
+  </si>
+  <si>
+    <t>Prisoners of War</t>
+  </si>
+  <si>
+    <t>Target ship: Roll a d6 and attach up to that many prisoners of war tokens to an equal amount of crew members. Crew members with a prisoners of war attached cannot tap.</t>
+  </si>
+  <si>
+    <t>All crew members that have a prisoners of war token attached are killed and sent to stasis</t>
+  </si>
+  <si>
+    <t>Prisoners Escaped!</t>
+  </si>
+  <si>
+    <t>Cleared Out</t>
+  </si>
+  <si>
+    <t>Target ship: Remove all crew attachments from target ship.</t>
+  </si>
+  <si>
+    <t>One at a time</t>
+  </si>
+  <si>
+    <t>Remove 1 crew attachment from 1 target crew member</t>
+  </si>
+  <si>
+    <t>Attach to ship: All crew members on ship can now tap: remove all crew attachments on tapped crew member</t>
+  </si>
+  <si>
+    <t>Seeing Stars Bar</t>
+  </si>
+  <si>
+    <t>Most ships have to have some form of entertainment and whats better than a bar to wipe yourself clean of all your troubles and responsibilities</t>
+  </si>
+  <si>
+    <t>Intergalactic Laxative</t>
+  </si>
+  <si>
+    <t>Target Ship: All crew members are tapped until the start of your next turn</t>
+  </si>
+  <si>
+    <t>Sometimes in space poo gets on the loose</t>
+  </si>
+  <si>
+    <t>Jerry's Space Diner</t>
+  </si>
+  <si>
+    <t>At the start of your turn draw 2 cards from either your strategy or crew deck and then place 1 card from your hand to the bottom of that cards deck.</t>
+  </si>
+  <si>
+    <t>Jerry's Diner is known for its gossips across the galaxy</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>Deal 500 damage to all ships</t>
+  </si>
+  <si>
+    <t>Galactic Diplomacy</t>
+  </si>
+  <si>
+    <t>At the start of each turn all players give 1 card from their hand to the player on their left</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -902,14 +1053,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -928,13 +1079,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Excel Services" refreshedDate="45013.926626157408" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="101" xr:uid="{B688DD9A-DD39-418C-87CC-4E60672EAA36}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="local-user" refreshedDate="45014.717974421299" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="123" xr:uid="{B688DD9A-DD39-418C-87CC-4E60672EAA36}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:Q200" sheet="Card Designs"/>
   </cacheSource>
   <cacheFields count="17">
     <cacheField name="Id" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="100"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="122"/>
     </cacheField>
     <cacheField name="Name" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -955,7 +1106,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="4"/>
     </cacheField>
     <cacheField name="Assault" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="4"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
     </cacheField>
     <cacheField name="X" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -1021,7 +1172,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="101">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="123">
   <r>
     <n v="1"/>
     <s v="Associate Scientist"/>
@@ -2923,6 +3074,424 @@
     <m/>
   </r>
   <r>
+    <n v="101"/>
+    <s v="Fighter Bot 2000"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+    <x v="2"/>
+    <s v="Uncommon"/>
+    <s v="Can only be tapped to use gun slot._x000a_When Using gun slot add an aditional 100 damage"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="102"/>
+    <s v="Knowing Shields"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="7"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Attach to crew: This crew member when used on gun slot add aditional 100 damage against a targets ships shield"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="103"/>
+    <s v="An extra hand"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <x v="7"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Attach to crew: This crew member can use one extra gun slot"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="104"/>
+    <s v="Wires Crossed"/>
+    <m/>
+    <n v="3"/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Rare"/>
+    <s v="Target ship: Switch targets ship shield with its hull"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="105"/>
+    <s v="Shield Booster"/>
+    <m/>
+    <m/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Target ship: Increase shield max by 200 and Restore 200 shield"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="106"/>
+    <s v="Flick the switch"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Common"/>
+    <s v="Target ship: Restore 200 shield"/>
+    <s v="Sometimes you just need to check everythings plugged in."/>
+    <m/>
+  </r>
+  <r>
+    <n v="107"/>
+    <s v="Unidentified Lifeform"/>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Rare"/>
+    <s v="Attach to ship: At the start of ship owners turn add a unidentified lifeform token to a empty crew slot. The token cannot be used on gun slots and has: Tap: remove unidentified lifeform and assigned ship takes 100 damage."/>
+    <s v="No one has ever known the true purpose of this disgusting lifeform but it just gets in the way"/>
+    <m/>
+  </r>
+  <r>
+    <n v="108"/>
+    <s v="Evolutionary Pod"/>
+    <m/>
+    <n v="3"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Rare"/>
+    <s v="Attach to ship: All unidentified lifeform tokens can now be used on a gun slot. When a unidentifed lifeform is used on a gun slot it is sacrified and deals an extra 400 to targeted ship"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="109"/>
+    <s v="Promotion!"/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Search your strategy deck for 1 crew card with a rank higher than 1 and place into your hand. Then shuffle your strategy deck."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="110"/>
+    <s v="Tractor Beam"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Steal target players ship upgrade from target enemy ship and attach to one of your ships"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="111"/>
+    <s v="Its in the stars"/>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Common"/>
+    <s v="Search your strategy deck for any card with converted cost of 4 or less and place into your hand. Then shuffle your strategy deck."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="112"/>
+    <s v="Even further beyond"/>
+    <m/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Search your strategy deck for any card with converted cost of 4 or less and immediately play without paying its cost. Then shuffle your strategy deck."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="113"/>
+    <s v="Fusion Reactor"/>
+    <m/>
+    <n v="1"/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Attach to ship: Increase ships maximum shield by 400 while this is attached. Restore shield back to full when this is first attached."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="114"/>
+    <s v="Prisoners of War"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="3"/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Target ship: Roll a d6 and attach up to that many prisoners of war tokens to an equal amount of crew members. Crew members with a prisoners of war attached cannot tap."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="115"/>
+    <s v="Prisoners Escaped!"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="5"/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="All crew members that have a prisoners of war token attached are killed and sent to stasis"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="116"/>
+    <s v="Cleared Out"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <x v="3"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Target ship: Remove all crew attachments from target ship."/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="117"/>
+    <s v="One at a time"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <x v="3"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Uncommon"/>
+    <s v="Remove 1 crew attachment from 1 target crew member"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="118"/>
+    <s v="Seeing Stars Bar"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="2"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Common"/>
+    <s v="Attach to ship: All crew members on ship can now tap: remove all crew attachments on tapped crew member"/>
+    <s v="Most ships have to have some form of entertainment and whats better than a bar to wipe yourself clean of all your troubles and responsibilities"/>
+    <m/>
+  </r>
+  <r>
+    <n v="119"/>
+    <s v="Intergalactic Laxative"/>
+    <m/>
+    <m/>
+    <m/>
+    <n v="3"/>
+    <m/>
+    <n v="3"/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Ultra Rare"/>
+    <s v="Target Ship: All crew members are tapped until the start of your next turn"/>
+    <s v="Sometimes in space poo gets on the loose"/>
+    <m/>
+  </r>
+  <r>
+    <n v="120"/>
+    <s v="Jerry's Space Diner"/>
+    <m/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Rare"/>
+    <s v="At the start of your turn draw 2 cards from either your strategy or crew deck and then place 1 card from your hand to the bottom of that cards deck."/>
+    <s v="Jerry's Diner is known for its gossips across the galaxy"/>
+    <m/>
+  </r>
+  <r>
+    <n v="121"/>
+    <s v="Black Hole"/>
+    <m/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <n v="2"/>
+    <m/>
+    <x v="1"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Rare"/>
+    <s v="Deal 500 damage to all ships"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <n v="122"/>
+    <s v="Galactic Diplomacy"/>
+    <m/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="4"/>
+    <x v="5"/>
+    <m/>
+    <x v="1"/>
+    <s v="Rare"/>
+    <s v="At the start of each turn all players give 1 card from their hand to the player on their left"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -2945,7 +3514,98 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56E0844B-B842-49FE-BAD9-C54D8B7F54DF}" name="PivotTable2" cacheId="34380" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95421989-C99E-48E6-8DB6-11F3B37CAE68}" name="PivotTable1" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="17">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
+      <items count="13">
+        <item x="8"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item m="1" x="10"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item m="1" x="11"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField compact="0" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Id" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56E0844B-B842-49FE-BAD9-C54D8B7F54DF}" name="PivotTable2" cacheId="36" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A17:E39" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="17">
     <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -3085,97 +3745,6 @@
     <i t="grand">
       <x/>
     </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Id" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95421989-C99E-48E6-8DB6-11F3B37CAE68}" name="PivotTable1" cacheId="34380" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="17">
-    <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" sortType="ascending">
-      <items count="13">
-        <item x="8"/>
-        <item x="5"/>
-        <item x="0"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item m="1" x="10"/>
-        <item x="6"/>
-        <item x="4"/>
-        <item m="1" x="11"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item h="1" x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" outline="0" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="9"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Id" fld="0" subtotal="count" baseField="0" baseItem="0"/>
@@ -3491,120 +4060,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0742F16-4937-4A8E-A8D7-41747212FF7D}">
   <dimension ref="A3:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" s="7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" s="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="B10" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="B11" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="B12" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B13" s="7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C18" t="s">
@@ -3617,280 +4186,280 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="6">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="6">
-        <v>1</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-      <c r="E21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="6">
-        <v>1</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="7">
         <v>2</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="6">
-        <v>1</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6">
-        <v>1</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="7">
         <v>5</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="7">
         <v>3</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="7">
         <v>4</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="7">
         <v>3</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="7">
         <v>4</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="7">
         <v>3</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="7">
         <v>4</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="7">
         <v>3</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="7">
         <v>4</v>
       </c>
-      <c r="D32" s="6">
-        <v>3</v>
-      </c>
-      <c r="E32" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="D32" s="7">
+        <v>4</v>
+      </c>
+      <c r="E32" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="6">
-        <v>1</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="6">
-        <v>1</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="6">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="6">
-        <v>1</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="6">
-        <v>1</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6">
-        <v>1</v>
-      </c>
-      <c r="E38" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="7">
         <v>34</v>
       </c>
-      <c r="D39" s="6">
-        <v>18</v>
-      </c>
-      <c r="E39" s="6">
-        <v>52</v>
+      <c r="D39" s="7">
+        <v>19</v>
+      </c>
+      <c r="E39" s="7">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -3900,16 +4469,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C49EA94B-2824-4AC9-A95E-59E2D4B44008}">
-  <dimension ref="A2:Q105"/>
+  <dimension ref="A2:Q127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="J106" sqref="J106"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B123" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
+      <selection pane="bottomRight" activeCell="K127" sqref="K127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -3927,25 +4496,25 @@
     <col min="17" max="17" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18.75">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -3998,7 +4567,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4028,7 +4597,7 @@
       </c>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:17" ht="30.75">
+    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4058,7 +4627,7 @@
       </c>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:17" ht="30.75">
+    <row r="8" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -4088,7 +4657,7 @@
       </c>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:17" ht="30.75">
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -4118,7 +4687,7 @@
       </c>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:17" ht="30.75">
+    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -4148,7 +4717,7 @@
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:17" ht="45.75">
+    <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -4178,7 +4747,7 @@
       </c>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:17" ht="45.75">
+    <row r="12" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -4208,7 +4777,7 @@
       </c>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:17" ht="30.75">
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -4238,7 +4807,7 @@
       </c>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -4268,7 +4837,7 @@
       </c>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:17" ht="30.75">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -4298,7 +4867,7 @@
       </c>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:17" ht="30.75">
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -4328,7 +4897,7 @@
       </c>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" ht="45.75">
+    <row r="17" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -4358,7 +4927,7 @@
       </c>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -4388,7 +4957,7 @@
       </c>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="30.75">
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -4418,7 +4987,7 @@
       </c>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" ht="30.75">
+    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
@@ -4448,7 +5017,7 @@
       </c>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" ht="76.5">
+    <row r="21" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
@@ -4478,7 +5047,7 @@
       </c>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -4508,7 +5077,7 @@
       </c>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" ht="30.75">
+    <row r="23" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -4538,7 +5107,7 @@
       </c>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" ht="30.75">
+    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
@@ -4568,7 +5137,7 @@
       </c>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" ht="45.75">
+    <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -4598,7 +5167,7 @@
       </c>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16" ht="76.5">
+    <row r="26" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
@@ -4619,7 +5188,7 @@
       </c>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16" ht="30.75">
+    <row r="27" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
@@ -4640,7 +5209,7 @@
       </c>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" ht="30.75">
+    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>23</v>
       </c>
@@ -4661,7 +5230,7 @@
       </c>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" ht="30.75">
+    <row r="29" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
@@ -4682,7 +5251,7 @@
       </c>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" ht="45.75">
+    <row r="30" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
@@ -4706,7 +5275,7 @@
       </c>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" ht="30.75">
+    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>26</v>
       </c>
@@ -4727,7 +5296,7 @@
       </c>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" ht="45.75">
+    <row r="32" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>27</v>
       </c>
@@ -4748,7 +5317,7 @@
       </c>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16" ht="30.75">
+    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
@@ -4769,7 +5338,7 @@
       </c>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="1:16" ht="30.75">
+    <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>29</v>
       </c>
@@ -4790,7 +5359,7 @@
       </c>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" ht="76.5">
+    <row r="35" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>30</v>
       </c>
@@ -4814,7 +5383,7 @@
       </c>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16" ht="45.75">
+    <row r="36" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>31</v>
       </c>
@@ -4835,7 +5404,7 @@
       </c>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="1:16" ht="30.75">
+    <row r="37" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>32</v>
       </c>
@@ -4856,7 +5425,7 @@
       </c>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="1:16" ht="45.75">
+    <row r="38" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>33</v>
       </c>
@@ -4879,7 +5448,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="30.75">
+    <row r="39" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>34</v>
       </c>
@@ -4902,7 +5471,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>35</v>
       </c>
@@ -4925,7 +5494,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="45.75">
+    <row r="41" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>36</v>
       </c>
@@ -4945,7 +5514,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>37</v>
       </c>
@@ -4965,7 +5534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="91.5">
+    <row r="43" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>38</v>
       </c>
@@ -4994,7 +5563,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="76.5">
+    <row r="44" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>39</v>
       </c>
@@ -5023,7 +5592,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="45.75">
+    <row r="45" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>40</v>
       </c>
@@ -5052,7 +5621,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="30.75">
+    <row r="46" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>41</v>
       </c>
@@ -5072,7 +5641,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>42</v>
       </c>
@@ -5092,7 +5661,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="45.75">
+    <row r="48" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>43</v>
       </c>
@@ -5112,7 +5681,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="45.75">
+    <row r="49" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>44</v>
       </c>
@@ -5132,7 +5701,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="45.75">
+    <row r="50" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>45</v>
       </c>
@@ -5152,7 +5721,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="45.75">
+    <row r="51" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>46</v>
       </c>
@@ -5172,7 +5741,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="45.75">
+    <row r="52" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>47</v>
       </c>
@@ -5198,7 +5767,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="76.5">
+    <row r="53" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>48</v>
       </c>
@@ -5218,7 +5787,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="91.5">
+    <row r="54" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>49</v>
       </c>
@@ -5247,7 +5816,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="45.75">
+    <row r="55" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>50</v>
       </c>
@@ -5267,7 +5836,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="91.5">
+    <row r="56" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>51</v>
       </c>
@@ -5287,7 +5856,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="60.75">
+    <row r="57" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>52</v>
       </c>
@@ -5307,7 +5876,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="30.75">
+    <row r="58" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>53</v>
       </c>
@@ -5327,7 +5896,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="60.75">
+    <row r="59" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>54</v>
       </c>
@@ -5350,7 +5919,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="60.75">
+    <row r="60" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>55</v>
       </c>
@@ -5379,7 +5948,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="60.75">
+    <row r="61" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>56</v>
       </c>
@@ -5408,7 +5977,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="60.75">
+    <row r="62" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>57</v>
       </c>
@@ -5437,7 +6006,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="60.75">
+    <row r="63" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>58</v>
       </c>
@@ -5466,7 +6035,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="60.75">
+    <row r="64" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>59</v>
       </c>
@@ -5495,7 +6064,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="91.5">
+    <row r="65" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>60</v>
       </c>
@@ -5524,7 +6093,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="76.5">
+    <row r="66" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>61</v>
       </c>
@@ -5553,7 +6122,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="76.5">
+    <row r="67" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>62</v>
       </c>
@@ -5582,7 +6151,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="76.5">
+    <row r="68" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>63</v>
       </c>
@@ -5611,7 +6180,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="76.5">
+    <row r="69" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>64</v>
       </c>
@@ -5640,7 +6209,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="91.5">
+    <row r="70" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>65</v>
       </c>
@@ -5669,7 +6238,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="76.5">
+    <row r="71" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>66</v>
       </c>
@@ -5698,7 +6267,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="76.5">
+    <row r="72" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>67</v>
       </c>
@@ -5727,7 +6296,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="76.5">
+    <row r="73" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>68</v>
       </c>
@@ -5756,7 +6325,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="76.5">
+    <row r="74" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>69</v>
       </c>
@@ -5785,7 +6354,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="45.75">
+    <row r="75" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>70</v>
       </c>
@@ -5826,7 +6395,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="76.5">
+    <row r="76" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>71</v>
       </c>
@@ -5867,7 +6436,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="60.75">
+    <row r="77" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>72</v>
       </c>
@@ -5890,7 +6459,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="45.75">
+    <row r="78" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>73</v>
       </c>
@@ -5910,7 +6479,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="106.5">
+    <row r="79" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>74</v>
       </c>
@@ -5933,7 +6502,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="45.75">
+    <row r="80" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>75</v>
       </c>
@@ -5956,7 +6525,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="45.75">
+    <row r="81" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>76</v>
       </c>
@@ -5976,7 +6545,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="45.75">
+    <row r="82" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>77</v>
       </c>
@@ -5999,7 +6568,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="91.5">
+    <row r="83" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>78</v>
       </c>
@@ -6028,7 +6597,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="76.5">
+    <row r="84" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>79</v>
       </c>
@@ -6057,7 +6626,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="76.5">
+    <row r="85" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>80</v>
       </c>
@@ -6086,7 +6655,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>81</v>
       </c>
@@ -6112,7 +6681,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="91.5">
+    <row r="87" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>82</v>
       </c>
@@ -6140,11 +6709,11 @@
       <c r="O87" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="P87" s="7" t="s">
+      <c r="P87" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="106.5">
+    <row r="88" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>83</v>
       </c>
@@ -6172,11 +6741,11 @@
       <c r="O88" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="P88" s="7" t="s">
+      <c r="P88" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="30.75">
+    <row r="89" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>84</v>
       </c>
@@ -6196,7 +6765,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>85</v>
       </c>
@@ -6216,7 +6785,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="30.75">
+    <row r="91" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>86</v>
       </c>
@@ -6239,7 +6808,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="45.75">
+    <row r="92" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>87</v>
       </c>
@@ -6271,7 +6840,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="76.5">
+    <row r="93" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>88</v>
       </c>
@@ -6295,7 +6864,7 @@
       </c>
       <c r="P93" s="2"/>
     </row>
-    <row r="94" spans="1:16" ht="91.5">
+    <row r="94" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>89</v>
       </c>
@@ -6332,11 +6901,11 @@
       <c r="O94" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="P94" s="7" t="s">
+      <c r="P94" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="30.75">
+    <row r="95" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>90</v>
       </c>
@@ -6365,7 +6934,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="45.75">
+    <row r="96" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>91</v>
       </c>
@@ -6394,7 +6963,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="45.75">
+    <row r="97" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>92</v>
       </c>
@@ -6423,7 +6992,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="30.75">
+    <row r="98" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>93</v>
       </c>
@@ -6452,7 +7021,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="76.5">
+    <row r="99" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>94</v>
       </c>
@@ -6472,7 +7041,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="76.5">
+    <row r="100" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>95</v>
       </c>
@@ -6492,7 +7061,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="91.5">
+    <row r="101" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>96</v>
       </c>
@@ -6512,7 +7081,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="76.5">
+    <row r="102" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>97</v>
       </c>
@@ -6532,7 +7101,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="76.5">
+    <row r="103" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>98</v>
       </c>
@@ -6552,7 +7121,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="60.75">
+    <row r="104" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>99</v>
       </c>
@@ -6572,7 +7141,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="45.75">
+    <row r="105" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>100</v>
       </c>
@@ -6593,6 +7162,509 @@
       </c>
       <c r="O105" s="2" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>101</v>
+      </c>
+      <c r="B106" t="s">
+        <v>241</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="J106" t="s">
+        <v>4</v>
+      </c>
+      <c r="K106" t="s">
+        <v>17</v>
+      </c>
+      <c r="L106">
+        <v>1</v>
+      </c>
+      <c r="M106" t="s">
+        <v>15</v>
+      </c>
+      <c r="N106" t="s">
+        <v>42</v>
+      </c>
+      <c r="O106" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>102</v>
+      </c>
+      <c r="B107" t="s">
+        <v>244</v>
+      </c>
+      <c r="F107">
+        <v>2</v>
+      </c>
+      <c r="J107" t="s">
+        <v>5</v>
+      </c>
+      <c r="N107" t="s">
+        <v>42</v>
+      </c>
+      <c r="O107" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>103</v>
+      </c>
+      <c r="B108" t="s">
+        <v>246</v>
+      </c>
+      <c r="F108">
+        <v>1</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+      <c r="J108" t="s">
+        <v>5</v>
+      </c>
+      <c r="N108" t="s">
+        <v>42</v>
+      </c>
+      <c r="O108" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>104</v>
+      </c>
+      <c r="B109" t="s">
+        <v>268</v>
+      </c>
+      <c r="D109">
+        <v>3</v>
+      </c>
+      <c r="E109">
+        <v>2</v>
+      </c>
+      <c r="J109" t="s">
+        <v>6</v>
+      </c>
+      <c r="N109" t="s">
+        <v>94</v>
+      </c>
+      <c r="O109" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>105</v>
+      </c>
+      <c r="B110" t="s">
+        <v>249</v>
+      </c>
+      <c r="E110">
+        <v>3</v>
+      </c>
+      <c r="J110" t="s">
+        <v>6</v>
+      </c>
+      <c r="N110" t="s">
+        <v>42</v>
+      </c>
+      <c r="O110" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>106</v>
+      </c>
+      <c r="B111" t="s">
+        <v>251</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="J111" t="s">
+        <v>6</v>
+      </c>
+      <c r="N111" t="s">
+        <v>35</v>
+      </c>
+      <c r="O111" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="P111" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>107</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <v>2</v>
+      </c>
+      <c r="J112" t="s">
+        <v>254</v>
+      </c>
+      <c r="N112" t="s">
+        <v>94</v>
+      </c>
+      <c r="O112" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="P112" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" ht="120" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>108</v>
+      </c>
+      <c r="B113" t="s">
+        <v>257</v>
+      </c>
+      <c r="D113">
+        <v>3</v>
+      </c>
+      <c r="E113">
+        <v>1</v>
+      </c>
+      <c r="J113" t="s">
+        <v>9</v>
+      </c>
+      <c r="N113" t="s">
+        <v>94</v>
+      </c>
+      <c r="O113" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>109</v>
+      </c>
+      <c r="B114" t="s">
+        <v>259</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="J114" t="s">
+        <v>6</v>
+      </c>
+      <c r="N114" t="s">
+        <v>42</v>
+      </c>
+      <c r="O114" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>110</v>
+      </c>
+      <c r="B115" t="s">
+        <v>260</v>
+      </c>
+      <c r="E115">
+        <v>1</v>
+      </c>
+      <c r="G115">
+        <v>1</v>
+      </c>
+      <c r="J115" t="s">
+        <v>6</v>
+      </c>
+      <c r="N115" t="s">
+        <v>42</v>
+      </c>
+      <c r="O115" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>111</v>
+      </c>
+      <c r="B116" t="s">
+        <v>262</v>
+      </c>
+      <c r="D116">
+        <v>2</v>
+      </c>
+      <c r="J116" t="s">
+        <v>6</v>
+      </c>
+      <c r="N116" t="s">
+        <v>35</v>
+      </c>
+      <c r="O116" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>112</v>
+      </c>
+      <c r="B117" t="s">
+        <v>264</v>
+      </c>
+      <c r="D117">
+        <v>4</v>
+      </c>
+      <c r="J117" t="s">
+        <v>6</v>
+      </c>
+      <c r="N117" t="s">
+        <v>42</v>
+      </c>
+      <c r="O117" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>113</v>
+      </c>
+      <c r="B118" t="s">
+        <v>266</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>3</v>
+      </c>
+      <c r="J118" t="s">
+        <v>9</v>
+      </c>
+      <c r="N118" t="s">
+        <v>42</v>
+      </c>
+      <c r="O118" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" ht="105" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>114</v>
+      </c>
+      <c r="B119" t="s">
+        <v>270</v>
+      </c>
+      <c r="H119">
+        <v>3</v>
+      </c>
+      <c r="J119" t="s">
+        <v>6</v>
+      </c>
+      <c r="N119" t="s">
+        <v>42</v>
+      </c>
+      <c r="O119" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>115</v>
+      </c>
+      <c r="B120" t="s">
+        <v>273</v>
+      </c>
+      <c r="H120">
+        <v>5</v>
+      </c>
+      <c r="J120" t="s">
+        <v>6</v>
+      </c>
+      <c r="N120" t="s">
+        <v>42</v>
+      </c>
+      <c r="O120" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>116</v>
+      </c>
+      <c r="B121" t="s">
+        <v>274</v>
+      </c>
+      <c r="F121">
+        <v>2</v>
+      </c>
+      <c r="H121">
+        <v>2</v>
+      </c>
+      <c r="J121" t="s">
+        <v>10</v>
+      </c>
+      <c r="N121" t="s">
+        <v>42</v>
+      </c>
+      <c r="O121" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>117</v>
+      </c>
+      <c r="B122" t="s">
+        <v>276</v>
+      </c>
+      <c r="H122">
+        <v>1</v>
+      </c>
+      <c r="J122" t="s">
+        <v>10</v>
+      </c>
+      <c r="N122" t="s">
+        <v>42</v>
+      </c>
+      <c r="O122" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>118</v>
+      </c>
+      <c r="B123" t="s">
+        <v>279</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <v>1</v>
+      </c>
+      <c r="J123" t="s">
+        <v>9</v>
+      </c>
+      <c r="N123" t="s">
+        <v>35</v>
+      </c>
+      <c r="O123" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="P123" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>119</v>
+      </c>
+      <c r="B124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F124">
+        <v>3</v>
+      </c>
+      <c r="H124">
+        <v>3</v>
+      </c>
+      <c r="J124" t="s">
+        <v>6</v>
+      </c>
+      <c r="N124" t="s">
+        <v>176</v>
+      </c>
+      <c r="O124" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P124" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" ht="90" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>120</v>
+      </c>
+      <c r="B125" t="s">
+        <v>284</v>
+      </c>
+      <c r="D125">
+        <v>3</v>
+      </c>
+      <c r="J125" t="s">
+        <v>8</v>
+      </c>
+      <c r="N125" t="s">
+        <v>94</v>
+      </c>
+      <c r="O125" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="P125" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>121</v>
+      </c>
+      <c r="B126" t="s">
+        <v>287</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>2</v>
+      </c>
+      <c r="F126">
+        <v>2</v>
+      </c>
+      <c r="G126">
+        <v>2</v>
+      </c>
+      <c r="H126">
+        <v>2</v>
+      </c>
+      <c r="J126" t="s">
+        <v>6</v>
+      </c>
+      <c r="N126" t="s">
+        <v>94</v>
+      </c>
+      <c r="O126" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="127" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>122</v>
+      </c>
+      <c r="B127" t="s">
+        <v>289</v>
+      </c>
+      <c r="D127">
+        <v>4</v>
+      </c>
+      <c r="J127" t="s">
+        <v>8</v>
+      </c>
+      <c r="N127" t="s">
+        <v>94</v>
+      </c>
+      <c r="O127" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done the final assets for the cards
Done final assets for cards, started some templates for the sizes and designs. Also slightly updated to a wording on a card or two in spready
</commit_message>
<xml_diff>
--- a/ShipCardsDesigns.xlsx
+++ b/ShipCardsDesigns.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MultiplayerGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{155D4A26-9B98-42E7-AE25-7FDB50088358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D997A7D2-CD5F-4CA1-905C-28F40E012245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,8 +34,8 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="358" r:id="rId11"/>
-    <pivotCache cacheId="359" r:id="rId12"/>
+    <pivotCache cacheId="469" r:id="rId11"/>
+    <pivotCache cacheId="470" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3710,7 +3710,7 @@
     <t>Lt. Chambers</t>
   </si>
   <si>
-    <t>Add the start of your Resource Allocation Phase, increment your Handling dice by 1</t>
+    <t>At the start of your Resource Allocation Phase, increment your Handling dice by 1</t>
   </si>
   <si>
     <t>Lt. Clarke</t>
@@ -5405,61 +5405,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5467,12 +5428,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5492,6 +5447,126 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5499,12 +5574,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5525,24 +5594,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5550,57 +5601,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -24469,7 +24469,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C17E6186-C211-45E3-BF98-94266063404B}" name="PivotTable2" cacheId="359" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C17E6186-C211-45E3-BF98-94266063404B}" name="PivotTable2" cacheId="470" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A19:G55" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="19">
     <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -24693,7 +24693,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91C0DB95-3F2E-49BF-A001-009CDB8468CF}" name="PivotTable1" cacheId="359" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91C0DB95-3F2E-49BF-A001-009CDB8468CF}" name="PivotTable1" cacheId="470" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="19">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -24796,7 +24796,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4889AD0-C894-4D73-8042-C68520653761}" name="PivotTable4" cacheId="358" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4889AD0-C894-4D73-8042-C68520653761}" name="PivotTable4" cacheId="469" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="E3:F9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
@@ -26027,8 +26027,8 @@
   <dimension ref="A2:S547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="R76" sqref="R76"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B289" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="Q295" sqref="Q295"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -33300,6 +33300,9 @@
       </c>
       <c r="M241" t="s">
         <v>29</v>
+      </c>
+      <c r="N241">
+        <v>1</v>
       </c>
       <c r="O241" t="s">
         <v>27</v>
@@ -40550,142 +40553,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:59" ht="15.75" thickBot="1">
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="83" t="s">
         <v>804</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
-      <c r="AH1" s="70"/>
-      <c r="AI1" s="70"/>
-      <c r="AJ1" s="70"/>
-      <c r="AK1" s="71"/>
-      <c r="AL1" s="69" t="s">
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
+      <c r="AG1" s="84"/>
+      <c r="AH1" s="84"/>
+      <c r="AI1" s="84"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="85"/>
+      <c r="AL1" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="AM1" s="70"/>
-      <c r="AN1" s="70"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="70"/>
-      <c r="AQ1" s="70"/>
-      <c r="AR1" s="70"/>
-      <c r="AS1" s="70"/>
-      <c r="AT1" s="70"/>
-      <c r="AU1" s="70"/>
-      <c r="AV1" s="70"/>
-      <c r="AW1" s="70"/>
-      <c r="AX1" s="70"/>
-      <c r="AY1" s="70"/>
-      <c r="AZ1" s="70"/>
-      <c r="BA1" s="70"/>
-      <c r="BB1" s="70"/>
-      <c r="BC1" s="71"/>
+      <c r="AM1" s="84"/>
+      <c r="AN1" s="84"/>
+      <c r="AO1" s="84"/>
+      <c r="AP1" s="84"/>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="84"/>
+      <c r="AS1" s="84"/>
+      <c r="AT1" s="84"/>
+      <c r="AU1" s="84"/>
+      <c r="AV1" s="84"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="84"/>
+      <c r="AY1" s="84"/>
+      <c r="AZ1" s="84"/>
+      <c r="BA1" s="84"/>
+      <c r="BB1" s="84"/>
+      <c r="BC1" s="85"/>
     </row>
     <row r="2" spans="2:59" ht="15.75" thickBot="1">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="78" t="s">
         <v>805</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
       <c r="G2" s="27"/>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="80" t="s">
         <v>806</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="76" t="s">
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="79" t="s">
         <v>807</v>
       </c>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="77" t="s">
+      <c r="O2" s="79"/>
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="80" t="s">
         <v>808</v>
       </c>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="76" t="s">
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="79" t="s">
         <v>809</v>
       </c>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="76"/>
-      <c r="AC2" s="76"/>
-      <c r="AD2" s="76"/>
-      <c r="AE2" s="76"/>
-      <c r="AF2" s="77" t="s">
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79"/>
+      <c r="AE2" s="79"/>
+      <c r="AF2" s="80" t="s">
         <v>810</v>
       </c>
-      <c r="AG2" s="76"/>
-      <c r="AH2" s="76"/>
-      <c r="AI2" s="76"/>
-      <c r="AJ2" s="76"/>
-      <c r="AK2" s="76"/>
-      <c r="AL2" s="75" t="s">
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="79"/>
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="78" t="s">
         <v>811</v>
       </c>
-      <c r="AM2" s="76"/>
-      <c r="AN2" s="76"/>
-      <c r="AO2" s="76"/>
-      <c r="AP2" s="76"/>
-      <c r="AQ2" s="76"/>
-      <c r="AR2" s="77" t="s">
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
+      <c r="AQ2" s="79"/>
+      <c r="AR2" s="80" t="s">
         <v>812</v>
       </c>
-      <c r="AS2" s="76"/>
-      <c r="AT2" s="76"/>
-      <c r="AU2" s="76"/>
-      <c r="AV2" s="76"/>
-      <c r="AW2" s="78"/>
-      <c r="AX2" s="76" t="s">
+      <c r="AS2" s="79"/>
+      <c r="AT2" s="79"/>
+      <c r="AU2" s="79"/>
+      <c r="AV2" s="79"/>
+      <c r="AW2" s="81"/>
+      <c r="AX2" s="79" t="s">
         <v>813</v>
       </c>
-      <c r="AY2" s="76"/>
-      <c r="AZ2" s="76"/>
-      <c r="BA2" s="76"/>
-      <c r="BB2" s="76"/>
-      <c r="BC2" s="127"/>
-      <c r="BE2" s="125" t="s">
+      <c r="AY2" s="79"/>
+      <c r="AZ2" s="79"/>
+      <c r="BA2" s="79"/>
+      <c r="BB2" s="79"/>
+      <c r="BC2" s="82"/>
+      <c r="BE2" s="86" t="s">
         <v>814</v>
       </c>
-      <c r="BF2" s="126"/>
+      <c r="BF2" s="87"/>
       <c r="BG2" s="23" t="s">
         <v>815</v>
       </c>
@@ -40697,12 +40700,12 @@
       <c r="C3" s="26">
         <v>21</v>
       </c>
-      <c r="D3" s="72" t="str">
+      <c r="D3" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(C3,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
       <c r="G3" s="10"/>
       <c r="H3" s="31" t="s">
         <v>816</v>
@@ -40710,110 +40713,110 @@
       <c r="I3" s="32">
         <v>21</v>
       </c>
-      <c r="J3" s="95" t="str">
+      <c r="J3" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(I3,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="96"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
       <c r="N3" s="10" t="s">
         <v>816</v>
       </c>
       <c r="O3" s="26">
         <v>66</v>
       </c>
-      <c r="P3" s="72" t="str">
+      <c r="P3" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(O3,TblCardDesign[ID],0),14)</f>
         <v>Rank: 3</v>
       </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="72"/>
-      <c r="S3" s="72"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
       <c r="T3" s="31" t="s">
         <v>816</v>
       </c>
       <c r="U3" s="32">
         <v>56</v>
       </c>
-      <c r="V3" s="95" t="str">
+      <c r="V3" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(U3,TblCardDesign[ID],0),14)</f>
         <v>Rank: 1</v>
       </c>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="96"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="64"/>
       <c r="Z3" s="10" t="s">
         <v>816</v>
       </c>
       <c r="AA3" s="26">
         <v>99</v>
       </c>
-      <c r="AB3" s="72" t="str">
+      <c r="AB3" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AA3,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="AC3" s="72"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="72"/>
+      <c r="AC3" s="77"/>
+      <c r="AD3" s="77"/>
+      <c r="AE3" s="77"/>
       <c r="AF3" s="31" t="s">
         <v>816</v>
       </c>
       <c r="AG3" s="32">
         <v>62</v>
       </c>
-      <c r="AH3" s="95" t="str">
+      <c r="AH3" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AG3,TblCardDesign[ID],0),14)</f>
         <v>Rank: 2</v>
       </c>
-      <c r="AI3" s="95"/>
-      <c r="AJ3" s="95"/>
-      <c r="AK3" s="96"/>
+      <c r="AI3" s="63"/>
+      <c r="AJ3" s="63"/>
+      <c r="AK3" s="64"/>
       <c r="AL3" s="10" t="s">
         <v>816</v>
       </c>
       <c r="AM3" s="26">
         <v>82</v>
       </c>
-      <c r="AN3" s="72" t="str">
+      <c r="AN3" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AM3,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="AO3" s="72"/>
-      <c r="AP3" s="72"/>
-      <c r="AQ3" s="72"/>
+      <c r="AO3" s="77"/>
+      <c r="AP3" s="77"/>
+      <c r="AQ3" s="77"/>
       <c r="AR3" s="31" t="s">
         <v>816</v>
       </c>
       <c r="AS3" s="32">
         <v>11</v>
       </c>
-      <c r="AT3" s="95" t="str">
+      <c r="AT3" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AS3,TblCardDesign[ID],0),14)</f>
         <v>Rank: 3</v>
       </c>
-      <c r="AU3" s="95"/>
-      <c r="AV3" s="95"/>
-      <c r="AW3" s="96"/>
+      <c r="AU3" s="63"/>
+      <c r="AV3" s="63"/>
+      <c r="AW3" s="64"/>
       <c r="AX3" s="31" t="s">
         <v>816</v>
       </c>
       <c r="AY3" s="32">
         <v>4</v>
       </c>
-      <c r="AZ3" s="95" t="str">
+      <c r="AZ3" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AY3,TblCardDesign[ID],0),14)</f>
         <v>Rank: 1</v>
       </c>
-      <c r="BA3" s="95"/>
-      <c r="BB3" s="95"/>
-      <c r="BC3" s="96"/>
+      <c r="BA3" s="63"/>
+      <c r="BB3" s="63"/>
+      <c r="BC3" s="64"/>
       <c r="BE3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="BF3" s="21">
         <f ca="1">RANDBETWEEN(1,BF5)</f>
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BG3" s="24" t="str">
         <f ca="1">UPPER(INDEX(TblCardDesign[#Data],MATCH(BF3,TblCardDesign[ID],0),2))</f>
@@ -40821,181 +40824,181 @@
       </c>
     </row>
     <row r="4" spans="2:59" ht="15.75" thickBot="1">
-      <c r="B4" s="73" t="str">
+      <c r="B4" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(C3,TblCardDesign[ID],0),3)</f>
         <v>The Great Nebula</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="73" t="str">
+      <c r="H4" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(I3,TblCardDesign[ID],0),3)</f>
         <v>The Great Nebula</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="72" t="str">
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="77" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(O3,TblCardDesign[ID],0),3)</f>
         <v>R Boop Bot</v>
       </c>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="73" t="str">
+      <c r="O4" s="77"/>
+      <c r="P4" s="77"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="77"/>
+      <c r="S4" s="77"/>
+      <c r="T4" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(U3,TblCardDesign[ID],0),3)</f>
         <v>R Bot</v>
       </c>
-      <c r="U4" s="72"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="72" t="str">
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="113"/>
+      <c r="Z4" s="77" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AA3,TblCardDesign[ID],0),3)</f>
         <v>Auto Cannon</v>
       </c>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
-      <c r="AC4" s="72"/>
-      <c r="AD4" s="72"/>
-      <c r="AE4" s="72"/>
-      <c r="AF4" s="73" t="str">
+      <c r="AA4" s="77"/>
+      <c r="AB4" s="77"/>
+      <c r="AC4" s="77"/>
+      <c r="AD4" s="77"/>
+      <c r="AE4" s="77"/>
+      <c r="AF4" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AG3,TblCardDesign[ID],0),3)</f>
         <v>B Bot Bot</v>
       </c>
-      <c r="AG4" s="72"/>
-      <c r="AH4" s="72"/>
-      <c r="AI4" s="72"/>
-      <c r="AJ4" s="72"/>
-      <c r="AK4" s="74"/>
-      <c r="AL4" s="72" t="str">
+      <c r="AG4" s="77"/>
+      <c r="AH4" s="77"/>
+      <c r="AI4" s="77"/>
+      <c r="AJ4" s="77"/>
+      <c r="AK4" s="113"/>
+      <c r="AL4" s="77" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AM3,TblCardDesign[ID],0),3)</f>
         <v>Adm. I.T.S Atrap</v>
       </c>
-      <c r="AM4" s="72"/>
-      <c r="AN4" s="72"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="73" t="str">
+      <c r="AM4" s="77"/>
+      <c r="AN4" s="77"/>
+      <c r="AO4" s="77"/>
+      <c r="AP4" s="77"/>
+      <c r="AQ4" s="77"/>
+      <c r="AR4" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AS3,TblCardDesign[ID],0),3)</f>
         <v>Chief Medical Officer</v>
       </c>
-      <c r="AS4" s="72"/>
-      <c r="AT4" s="72"/>
-      <c r="AU4" s="72"/>
-      <c r="AV4" s="72"/>
-      <c r="AW4" s="74"/>
-      <c r="AX4" s="73" t="str">
+      <c r="AS4" s="77"/>
+      <c r="AT4" s="77"/>
+      <c r="AU4" s="77"/>
+      <c r="AV4" s="77"/>
+      <c r="AW4" s="113"/>
+      <c r="AX4" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AY3,TblCardDesign[ID],0),3)</f>
         <v>Mad Scientist</v>
       </c>
-      <c r="AY4" s="72"/>
-      <c r="AZ4" s="72"/>
-      <c r="BA4" s="72"/>
-      <c r="BB4" s="72"/>
-      <c r="BC4" s="74"/>
+      <c r="AY4" s="77"/>
+      <c r="AZ4" s="77"/>
+      <c r="BA4" s="77"/>
+      <c r="BB4" s="77"/>
+      <c r="BC4" s="113"/>
       <c r="BE4" s="20" t="s">
         <v>804</v>
       </c>
       <c r="BF4" s="22">
         <f ca="1">RANDBETWEEN(1,BF5)</f>
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="BG4" s="25" t="str">
         <f ca="1">UPPER(INDEX(TblCardDesign[#Data],MATCH(BF4,TblCardDesign[ID],0),2))</f>
-        <v>STRATEGY</v>
+        <v>CREW</v>
       </c>
     </row>
     <row r="5" spans="2:59">
-      <c r="B5" s="112" t="str">
+      <c r="B5" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(C3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="112" t="str">
+      <c r="H5" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(I3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="113" t="str">
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="115" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(O3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="113"/>
-      <c r="T5" s="112" t="str">
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="115"/>
+      <c r="R5" s="115"/>
+      <c r="S5" s="115"/>
+      <c r="T5" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(U3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="U5" s="113"/>
-      <c r="V5" s="113"/>
-      <c r="W5" s="113"/>
-      <c r="X5" s="113"/>
-      <c r="Y5" s="114"/>
-      <c r="Z5" s="113" t="str">
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="115"/>
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="115" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AA3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="112" t="str">
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="115"/>
+      <c r="AF5" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AG3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AG5" s="113"/>
-      <c r="AH5" s="113"/>
-      <c r="AI5" s="113"/>
-      <c r="AJ5" s="113"/>
-      <c r="AK5" s="114"/>
-      <c r="AL5" s="113" t="str">
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="115"/>
+      <c r="AI5" s="115"/>
+      <c r="AJ5" s="115"/>
+      <c r="AK5" s="116"/>
+      <c r="AL5" s="115" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AM3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AM5" s="113"/>
-      <c r="AN5" s="113"/>
-      <c r="AO5" s="113"/>
-      <c r="AP5" s="113"/>
-      <c r="AQ5" s="113"/>
-      <c r="AR5" s="112" t="str">
+      <c r="AM5" s="115"/>
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AS3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AS5" s="113"/>
-      <c r="AT5" s="113"/>
-      <c r="AU5" s="113"/>
-      <c r="AV5" s="113"/>
-      <c r="AW5" s="114"/>
-      <c r="AX5" s="112" t="str">
+      <c r="AS5" s="115"/>
+      <c r="AT5" s="115"/>
+      <c r="AU5" s="115"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="116"/>
+      <c r="AX5" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AY3,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AY5" s="113"/>
-      <c r="AZ5" s="113"/>
-      <c r="BA5" s="113"/>
-      <c r="BB5" s="113"/>
-      <c r="BC5" s="114"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="115"/>
+      <c r="BA5" s="115"/>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="116"/>
       <c r="BE5" t="s">
         <v>817</v>
       </c>
@@ -41387,226 +41390,226 @@
       </c>
     </row>
     <row r="8" spans="2:59">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="72" t="s">
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="113"/>
+      <c r="N8" s="77" t="s">
         <v>824</v>
       </c>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="73" t="s">
+      <c r="O8" s="77"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
+      <c r="S8" s="77"/>
+      <c r="T8" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="72"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="72" t="s">
+      <c r="U8" s="77"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="77"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="113"/>
+      <c r="Z8" s="77" t="s">
         <v>824</v>
       </c>
-      <c r="AA8" s="72"/>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="72"/>
-      <c r="AD8" s="72"/>
-      <c r="AE8" s="72"/>
-      <c r="AF8" s="73" t="s">
+      <c r="AA8" s="77"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="77"/>
+      <c r="AD8" s="77"/>
+      <c r="AE8" s="77"/>
+      <c r="AF8" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="AG8" s="72"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="72"/>
-      <c r="AJ8" s="72"/>
-      <c r="AK8" s="74"/>
-      <c r="AL8" s="72" t="s">
+      <c r="AG8" s="77"/>
+      <c r="AH8" s="77"/>
+      <c r="AI8" s="77"/>
+      <c r="AJ8" s="77"/>
+      <c r="AK8" s="113"/>
+      <c r="AL8" s="77" t="s">
         <v>824</v>
       </c>
-      <c r="AM8" s="72"/>
-      <c r="AN8" s="72"/>
-      <c r="AO8" s="72"/>
-      <c r="AP8" s="72"/>
-      <c r="AQ8" s="72"/>
-      <c r="AR8" s="79" t="s">
+      <c r="AM8" s="77"/>
+      <c r="AN8" s="77"/>
+      <c r="AO8" s="77"/>
+      <c r="AP8" s="77"/>
+      <c r="AQ8" s="77"/>
+      <c r="AR8" s="109" t="s">
         <v>824</v>
       </c>
-      <c r="AS8" s="80"/>
-      <c r="AT8" s="80"/>
-      <c r="AU8" s="80"/>
-      <c r="AV8" s="80"/>
-      <c r="AW8" s="81"/>
-      <c r="AX8" s="73" t="s">
+      <c r="AS8" s="110"/>
+      <c r="AT8" s="110"/>
+      <c r="AU8" s="110"/>
+      <c r="AV8" s="110"/>
+      <c r="AW8" s="111"/>
+      <c r="AX8" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="AY8" s="72"/>
-      <c r="AZ8" s="72"/>
-      <c r="BA8" s="72"/>
-      <c r="BB8" s="72"/>
-      <c r="BC8" s="74"/>
+      <c r="AY8" s="77"/>
+      <c r="AZ8" s="77"/>
+      <c r="BA8" s="77"/>
+      <c r="BB8" s="77"/>
+      <c r="BC8" s="113"/>
     </row>
     <row r="9" spans="2:59" ht="15" customHeight="1" thickBot="1">
-      <c r="B9" s="63" t="str">
+      <c r="B9" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(C3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Look at the top 3 cards of your Strategy Deck, put 2 Event cards into your hand and the rest into the junkyard</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="63" t="str">
+      <c r="H9" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(I3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Look at the top 3 cards of your Strategy Deck, put 2 Event cards into your hand and the rest into the junkyard</v>
       </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="64" t="str">
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="89"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="89" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(O3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Sacrifice 1 Medic Tier 2
 Robot can't be used for gun slots.
 Engage: Medic + 3
 Engage: Repair ship by 100</v>
       </c>
-      <c r="O9" s="64"/>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="63" t="str">
+      <c r="O9" s="89"/>
+      <c r="P9" s="89"/>
+      <c r="Q9" s="89"/>
+      <c r="R9" s="89"/>
+      <c r="S9" s="89"/>
+      <c r="T9" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(U3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Robot can't be used for gun slots.
 Engage: Medic + 1
 Engage: Repair ship by 100</v>
       </c>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="64" t="str">
+      <c r="U9" s="89"/>
+      <c r="V9" s="89"/>
+      <c r="W9" s="89"/>
+      <c r="X9" s="89"/>
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="89" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AA3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Attach to Ship: When this ship is targetted by enemy ship gun slots, deal 200 damage to that enemy ship</v>
       </c>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="64"/>
-      <c r="AC9" s="64"/>
-      <c r="AD9" s="64"/>
-      <c r="AE9" s="64"/>
-      <c r="AF9" s="63" t="str">
+      <c r="AA9" s="89"/>
+      <c r="AB9" s="89"/>
+      <c r="AC9" s="89"/>
+      <c r="AD9" s="89"/>
+      <c r="AE9" s="89"/>
+      <c r="AF9" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AG3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Sacrifice 1 Handling Tier 1
 Robot can't be used for gun slots.
 Engage: Handling + 2
 Engage: Repair ship by 100</v>
       </c>
-      <c r="AG9" s="64"/>
-      <c r="AH9" s="64"/>
-      <c r="AI9" s="64"/>
-      <c r="AJ9" s="64"/>
-      <c r="AK9" s="65"/>
-      <c r="AL9" s="64" t="str">
+      <c r="AG9" s="89"/>
+      <c r="AH9" s="89"/>
+      <c r="AI9" s="89"/>
+      <c r="AJ9" s="89"/>
+      <c r="AK9" s="90"/>
+      <c r="AL9" s="89" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AM3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Provides 1x Frigate ship when your Capital ship is destroyed, fill crew slots with any crew that wouldve died up to maximum Frigate crew slots.</v>
       </c>
-      <c r="AM9" s="64"/>
-      <c r="AN9" s="64"/>
-      <c r="AO9" s="64"/>
-      <c r="AP9" s="64"/>
-      <c r="AQ9" s="64"/>
-      <c r="AR9" s="63" t="str">
+      <c r="AM9" s="89"/>
+      <c r="AN9" s="89"/>
+      <c r="AO9" s="89"/>
+      <c r="AP9" s="89"/>
+      <c r="AQ9" s="89"/>
+      <c r="AR9" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AS3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Sacrifice 1 Medic Tier 2
 Engage: Medical + 3</v>
       </c>
-      <c r="AS9" s="64"/>
-      <c r="AT9" s="64"/>
-      <c r="AU9" s="64"/>
-      <c r="AV9" s="64"/>
-      <c r="AW9" s="65"/>
-      <c r="AX9" s="63" t="str">
+      <c r="AS9" s="89"/>
+      <c r="AT9" s="89"/>
+      <c r="AU9" s="89"/>
+      <c r="AV9" s="89"/>
+      <c r="AW9" s="90"/>
+      <c r="AX9" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AY3,TblCardDesign[ID],0),'Card Designs'!Q3)</f>
         <v>Engage: Discard 1 strategy card from your hand, if you do then Research + 2</v>
       </c>
-      <c r="AY9" s="64"/>
-      <c r="AZ9" s="64"/>
-      <c r="BA9" s="64"/>
-      <c r="BB9" s="64"/>
-      <c r="BC9" s="65"/>
+      <c r="AY9" s="89"/>
+      <c r="AZ9" s="89"/>
+      <c r="BA9" s="89"/>
+      <c r="BB9" s="89"/>
+      <c r="BC9" s="90"/>
     </row>
     <row r="10" spans="2:59" ht="30.75" thickBot="1">
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="89"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="63"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="64"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="64"/>
-      <c r="AA10" s="64"/>
-      <c r="AB10" s="64"/>
-      <c r="AC10" s="64"/>
-      <c r="AD10" s="64"/>
-      <c r="AE10" s="64"/>
-      <c r="AF10" s="63"/>
-      <c r="AG10" s="64"/>
-      <c r="AH10" s="64"/>
-      <c r="AI10" s="64"/>
-      <c r="AJ10" s="64"/>
-      <c r="AK10" s="65"/>
-      <c r="AL10" s="64"/>
-      <c r="AM10" s="64"/>
-      <c r="AN10" s="64"/>
-      <c r="AO10" s="64"/>
-      <c r="AP10" s="64"/>
-      <c r="AQ10" s="64"/>
-      <c r="AR10" s="63"/>
-      <c r="AS10" s="64"/>
-      <c r="AT10" s="64"/>
-      <c r="AU10" s="64"/>
-      <c r="AV10" s="64"/>
-      <c r="AW10" s="65"/>
-      <c r="AX10" s="63"/>
-      <c r="AY10" s="64"/>
-      <c r="AZ10" s="64"/>
-      <c r="BA10" s="64"/>
-      <c r="BB10" s="64"/>
-      <c r="BC10" s="65"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="89"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="89"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="88"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="90"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+      <c r="AB10" s="89"/>
+      <c r="AC10" s="89"/>
+      <c r="AD10" s="89"/>
+      <c r="AE10" s="89"/>
+      <c r="AF10" s="88"/>
+      <c r="AG10" s="89"/>
+      <c r="AH10" s="89"/>
+      <c r="AI10" s="89"/>
+      <c r="AJ10" s="89"/>
+      <c r="AK10" s="90"/>
+      <c r="AL10" s="89"/>
+      <c r="AM10" s="89"/>
+      <c r="AN10" s="89"/>
+      <c r="AO10" s="89"/>
+      <c r="AP10" s="89"/>
+      <c r="AQ10" s="89"/>
+      <c r="AR10" s="88"/>
+      <c r="AS10" s="89"/>
+      <c r="AT10" s="89"/>
+      <c r="AU10" s="89"/>
+      <c r="AV10" s="89"/>
+      <c r="AW10" s="90"/>
+      <c r="AX10" s="88"/>
+      <c r="AY10" s="89"/>
+      <c r="AZ10" s="89"/>
+      <c r="BA10" s="89"/>
+      <c r="BB10" s="89"/>
+      <c r="BC10" s="90"/>
       <c r="BE10" s="49" t="s">
         <v>825</v>
       </c>
@@ -41619,351 +41622,351 @@
       </c>
     </row>
     <row r="11" spans="2:59">
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="64"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="64"/>
-      <c r="O11" s="64"/>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="64"/>
-      <c r="S11" s="64"/>
-      <c r="T11" s="63"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="64"/>
-      <c r="X11" s="64"/>
-      <c r="Y11" s="65"/>
-      <c r="Z11" s="64"/>
-      <c r="AA11" s="64"/>
-      <c r="AB11" s="64"/>
-      <c r="AC11" s="64"/>
-      <c r="AD11" s="64"/>
-      <c r="AE11" s="64"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="64"/>
-      <c r="AH11" s="64"/>
-      <c r="AI11" s="64"/>
-      <c r="AJ11" s="64"/>
-      <c r="AK11" s="65"/>
-      <c r="AL11" s="64"/>
-      <c r="AM11" s="64"/>
-      <c r="AN11" s="64"/>
-      <c r="AO11" s="64"/>
-      <c r="AP11" s="64"/>
-      <c r="AQ11" s="64"/>
-      <c r="AR11" s="63"/>
-      <c r="AS11" s="64"/>
-      <c r="AT11" s="64"/>
-      <c r="AU11" s="64"/>
-      <c r="AV11" s="64"/>
-      <c r="AW11" s="65"/>
-      <c r="AX11" s="63"/>
-      <c r="AY11" s="64"/>
-      <c r="AZ11" s="64"/>
-      <c r="BA11" s="64"/>
-      <c r="BB11" s="64"/>
-      <c r="BC11" s="65"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="89"/>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="88"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="90"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+      <c r="AB11" s="89"/>
+      <c r="AC11" s="89"/>
+      <c r="AD11" s="89"/>
+      <c r="AE11" s="89"/>
+      <c r="AF11" s="88"/>
+      <c r="AG11" s="89"/>
+      <c r="AH11" s="89"/>
+      <c r="AI11" s="89"/>
+      <c r="AJ11" s="89"/>
+      <c r="AK11" s="90"/>
+      <c r="AL11" s="89"/>
+      <c r="AM11" s="89"/>
+      <c r="AN11" s="89"/>
+      <c r="AO11" s="89"/>
+      <c r="AP11" s="89"/>
+      <c r="AQ11" s="89"/>
+      <c r="AR11" s="88"/>
+      <c r="AS11" s="89"/>
+      <c r="AT11" s="89"/>
+      <c r="AU11" s="89"/>
+      <c r="AV11" s="89"/>
+      <c r="AW11" s="90"/>
+      <c r="AX11" s="88"/>
+      <c r="AY11" s="89"/>
+      <c r="AZ11" s="89"/>
+      <c r="BA11" s="89"/>
+      <c r="BB11" s="89"/>
+      <c r="BC11" s="90"/>
     </row>
     <row r="12" spans="2:59">
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="89"/>
+      <c r="F12" s="89"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="64"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="64"/>
-      <c r="O12" s="64"/>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="64"/>
-      <c r="T12" s="63"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="64"/>
-      <c r="X12" s="64"/>
-      <c r="Y12" s="65"/>
-      <c r="Z12" s="64"/>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="64"/>
-      <c r="AC12" s="64"/>
-      <c r="AD12" s="64"/>
-      <c r="AE12" s="64"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="64"/>
-      <c r="AH12" s="64"/>
-      <c r="AI12" s="64"/>
-      <c r="AJ12" s="64"/>
-      <c r="AK12" s="65"/>
-      <c r="AL12" s="64"/>
-      <c r="AM12" s="64"/>
-      <c r="AN12" s="64"/>
-      <c r="AO12" s="64"/>
-      <c r="AP12" s="64"/>
-      <c r="AQ12" s="64"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="64"/>
-      <c r="AT12" s="64"/>
-      <c r="AU12" s="64"/>
-      <c r="AV12" s="64"/>
-      <c r="AW12" s="65"/>
-      <c r="AX12" s="63"/>
-      <c r="AY12" s="64"/>
-      <c r="AZ12" s="64"/>
-      <c r="BA12" s="64"/>
-      <c r="BB12" s="64"/>
-      <c r="BC12" s="65"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="89"/>
+      <c r="K12" s="89"/>
+      <c r="L12" s="89"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="88"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="90"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+      <c r="AB12" s="89"/>
+      <c r="AC12" s="89"/>
+      <c r="AD12" s="89"/>
+      <c r="AE12" s="89"/>
+      <c r="AF12" s="88"/>
+      <c r="AG12" s="89"/>
+      <c r="AH12" s="89"/>
+      <c r="AI12" s="89"/>
+      <c r="AJ12" s="89"/>
+      <c r="AK12" s="90"/>
+      <c r="AL12" s="89"/>
+      <c r="AM12" s="89"/>
+      <c r="AN12" s="89"/>
+      <c r="AO12" s="89"/>
+      <c r="AP12" s="89"/>
+      <c r="AQ12" s="89"/>
+      <c r="AR12" s="88"/>
+      <c r="AS12" s="89"/>
+      <c r="AT12" s="89"/>
+      <c r="AU12" s="89"/>
+      <c r="AV12" s="89"/>
+      <c r="AW12" s="90"/>
+      <c r="AX12" s="88"/>
+      <c r="AY12" s="89"/>
+      <c r="AZ12" s="89"/>
+      <c r="BA12" s="89"/>
+      <c r="BB12" s="89"/>
+      <c r="BC12" s="90"/>
     </row>
     <row r="13" spans="2:59">
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="89"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64"/>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="63"/>
-      <c r="U13" s="64"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="64"/>
-      <c r="X13" s="64"/>
-      <c r="Y13" s="65"/>
-      <c r="Z13" s="64"/>
-      <c r="AA13" s="64"/>
-      <c r="AB13" s="64"/>
-      <c r="AC13" s="64"/>
-      <c r="AD13" s="64"/>
-      <c r="AE13" s="64"/>
-      <c r="AF13" s="63"/>
-      <c r="AG13" s="64"/>
-      <c r="AH13" s="64"/>
-      <c r="AI13" s="64"/>
-      <c r="AJ13" s="64"/>
-      <c r="AK13" s="65"/>
-      <c r="AL13" s="64"/>
-      <c r="AM13" s="64"/>
-      <c r="AN13" s="64"/>
-      <c r="AO13" s="64"/>
-      <c r="AP13" s="64"/>
-      <c r="AQ13" s="64"/>
-      <c r="AR13" s="63"/>
-      <c r="AS13" s="64"/>
-      <c r="AT13" s="64"/>
-      <c r="AU13" s="64"/>
-      <c r="AV13" s="64"/>
-      <c r="AW13" s="65"/>
-      <c r="AX13" s="63"/>
-      <c r="AY13" s="64"/>
-      <c r="AZ13" s="64"/>
-      <c r="BA13" s="64"/>
-      <c r="BB13" s="64"/>
-      <c r="BC13" s="65"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="89"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="88"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
+      <c r="X13" s="89"/>
+      <c r="Y13" s="90"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
+      <c r="AB13" s="89"/>
+      <c r="AC13" s="89"/>
+      <c r="AD13" s="89"/>
+      <c r="AE13" s="89"/>
+      <c r="AF13" s="88"/>
+      <c r="AG13" s="89"/>
+      <c r="AH13" s="89"/>
+      <c r="AI13" s="89"/>
+      <c r="AJ13" s="89"/>
+      <c r="AK13" s="90"/>
+      <c r="AL13" s="89"/>
+      <c r="AM13" s="89"/>
+      <c r="AN13" s="89"/>
+      <c r="AO13" s="89"/>
+      <c r="AP13" s="89"/>
+      <c r="AQ13" s="89"/>
+      <c r="AR13" s="88"/>
+      <c r="AS13" s="89"/>
+      <c r="AT13" s="89"/>
+      <c r="AU13" s="89"/>
+      <c r="AV13" s="89"/>
+      <c r="AW13" s="90"/>
+      <c r="AX13" s="88"/>
+      <c r="AY13" s="89"/>
+      <c r="AZ13" s="89"/>
+      <c r="BA13" s="89"/>
+      <c r="BB13" s="89"/>
+      <c r="BC13" s="90"/>
     </row>
     <row r="14" spans="2:59">
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="64"/>
-      <c r="O14" s="64"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64"/>
-      <c r="R14" s="64"/>
-      <c r="S14" s="64"/>
-      <c r="T14" s="63"/>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="64"/>
-      <c r="Y14" s="65"/>
-      <c r="Z14" s="64"/>
-      <c r="AA14" s="64"/>
-      <c r="AB14" s="64"/>
-      <c r="AC14" s="64"/>
-      <c r="AD14" s="64"/>
-      <c r="AE14" s="64"/>
-      <c r="AF14" s="63"/>
-      <c r="AG14" s="64"/>
-      <c r="AH14" s="64"/>
-      <c r="AI14" s="64"/>
-      <c r="AJ14" s="64"/>
-      <c r="AK14" s="65"/>
-      <c r="AL14" s="64"/>
-      <c r="AM14" s="64"/>
-      <c r="AN14" s="64"/>
-      <c r="AO14" s="64"/>
-      <c r="AP14" s="64"/>
-      <c r="AQ14" s="64"/>
-      <c r="AR14" s="63"/>
-      <c r="AS14" s="64"/>
-      <c r="AT14" s="64"/>
-      <c r="AU14" s="64"/>
-      <c r="AV14" s="64"/>
-      <c r="AW14" s="65"/>
-      <c r="AX14" s="63"/>
-      <c r="AY14" s="64"/>
-      <c r="AZ14" s="64"/>
-      <c r="BA14" s="64"/>
-      <c r="BB14" s="64"/>
-      <c r="BC14" s="65"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="89"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="89"/>
+      <c r="L14" s="89"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="88"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="90"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+      <c r="AB14" s="89"/>
+      <c r="AC14" s="89"/>
+      <c r="AD14" s="89"/>
+      <c r="AE14" s="89"/>
+      <c r="AF14" s="88"/>
+      <c r="AG14" s="89"/>
+      <c r="AH14" s="89"/>
+      <c r="AI14" s="89"/>
+      <c r="AJ14" s="89"/>
+      <c r="AK14" s="90"/>
+      <c r="AL14" s="89"/>
+      <c r="AM14" s="89"/>
+      <c r="AN14" s="89"/>
+      <c r="AO14" s="89"/>
+      <c r="AP14" s="89"/>
+      <c r="AQ14" s="89"/>
+      <c r="AR14" s="88"/>
+      <c r="AS14" s="89"/>
+      <c r="AT14" s="89"/>
+      <c r="AU14" s="89"/>
+      <c r="AV14" s="89"/>
+      <c r="AW14" s="90"/>
+      <c r="AX14" s="88"/>
+      <c r="AY14" s="89"/>
+      <c r="AZ14" s="89"/>
+      <c r="BA14" s="89"/>
+      <c r="BB14" s="89"/>
+      <c r="BC14" s="90"/>
     </row>
     <row r="15" spans="2:59" ht="15.75" thickBot="1">
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="67"/>
-      <c r="S15" s="67"/>
-      <c r="T15" s="66"/>
-      <c r="U15" s="67"/>
-      <c r="V15" s="67"/>
-      <c r="W15" s="67"/>
-      <c r="X15" s="67"/>
-      <c r="Y15" s="68"/>
-      <c r="Z15" s="67"/>
-      <c r="AA15" s="67"/>
-      <c r="AB15" s="67"/>
-      <c r="AC15" s="67"/>
-      <c r="AD15" s="67"/>
-      <c r="AE15" s="67"/>
-      <c r="AF15" s="66"/>
-      <c r="AG15" s="67"/>
-      <c r="AH15" s="67"/>
-      <c r="AI15" s="67"/>
-      <c r="AJ15" s="67"/>
-      <c r="AK15" s="68"/>
-      <c r="AL15" s="67"/>
-      <c r="AM15" s="67"/>
-      <c r="AN15" s="67"/>
-      <c r="AO15" s="67"/>
-      <c r="AP15" s="67"/>
-      <c r="AQ15" s="67"/>
-      <c r="AR15" s="66"/>
-      <c r="AS15" s="67"/>
-      <c r="AT15" s="67"/>
-      <c r="AU15" s="67"/>
-      <c r="AV15" s="67"/>
-      <c r="AW15" s="68"/>
-      <c r="AX15" s="66"/>
-      <c r="AY15" s="67"/>
-      <c r="AZ15" s="67"/>
-      <c r="BA15" s="67"/>
-      <c r="BB15" s="67"/>
-      <c r="BC15" s="68"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="93"/>
+      <c r="N15" s="92"/>
+      <c r="O15" s="92"/>
+      <c r="P15" s="92"/>
+      <c r="Q15" s="92"/>
+      <c r="R15" s="92"/>
+      <c r="S15" s="92"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="92"/>
+      <c r="V15" s="92"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="92"/>
+      <c r="Y15" s="93"/>
+      <c r="Z15" s="92"/>
+      <c r="AA15" s="92"/>
+      <c r="AB15" s="92"/>
+      <c r="AC15" s="92"/>
+      <c r="AD15" s="92"/>
+      <c r="AE15" s="92"/>
+      <c r="AF15" s="91"/>
+      <c r="AG15" s="92"/>
+      <c r="AH15" s="92"/>
+      <c r="AI15" s="92"/>
+      <c r="AJ15" s="92"/>
+      <c r="AK15" s="93"/>
+      <c r="AL15" s="92"/>
+      <c r="AM15" s="92"/>
+      <c r="AN15" s="92"/>
+      <c r="AO15" s="92"/>
+      <c r="AP15" s="92"/>
+      <c r="AQ15" s="92"/>
+      <c r="AR15" s="91"/>
+      <c r="AS15" s="92"/>
+      <c r="AT15" s="92"/>
+      <c r="AU15" s="92"/>
+      <c r="AV15" s="92"/>
+      <c r="AW15" s="93"/>
+      <c r="AX15" s="91"/>
+      <c r="AY15" s="92"/>
+      <c r="AZ15" s="92"/>
+      <c r="BA15" s="92"/>
+      <c r="BB15" s="92"/>
+      <c r="BC15" s="93"/>
     </row>
     <row r="16" spans="2:59" ht="15.75" thickBot="1">
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="120" t="s">
         <v>826</v>
       </c>
-      <c r="C16" s="98"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="98"/>
-      <c r="J16" s="98"/>
-      <c r="K16" s="98"/>
-      <c r="L16" s="98"/>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
-      <c r="O16" s="98"/>
-      <c r="P16" s="98"/>
-      <c r="Q16" s="98"/>
-      <c r="R16" s="98"/>
-      <c r="S16" s="98"/>
-      <c r="T16" s="98"/>
-      <c r="U16" s="98"/>
-      <c r="V16" s="98"/>
-      <c r="W16" s="98"/>
-      <c r="X16" s="98"/>
-      <c r="Y16" s="98"/>
-      <c r="Z16" s="98"/>
-      <c r="AA16" s="98"/>
-      <c r="AB16" s="98"/>
-      <c r="AC16" s="98"/>
-      <c r="AD16" s="98"/>
-      <c r="AE16" s="98"/>
-      <c r="AF16" s="98"/>
-      <c r="AG16" s="98"/>
-      <c r="AH16" s="98"/>
-      <c r="AI16" s="98"/>
-      <c r="AJ16" s="98"/>
-      <c r="AK16" s="98"/>
-      <c r="AL16" s="98"/>
-      <c r="AM16" s="98"/>
-      <c r="AN16" s="98"/>
-      <c r="AO16" s="98"/>
-      <c r="AP16" s="98"/>
-      <c r="AQ16" s="98"/>
-      <c r="AR16" s="98"/>
-      <c r="AS16" s="98"/>
-      <c r="AT16" s="98"/>
-      <c r="AU16" s="98"/>
-      <c r="AV16" s="98"/>
-      <c r="AW16" s="98"/>
-      <c r="AX16" s="98"/>
-      <c r="AY16" s="98"/>
-      <c r="AZ16" s="98"/>
-      <c r="BA16" s="98"/>
-      <c r="BB16" s="98"/>
-      <c r="BC16" s="99"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="121"/>
+      <c r="Q16" s="121"/>
+      <c r="R16" s="121"/>
+      <c r="S16" s="121"/>
+      <c r="T16" s="121"/>
+      <c r="U16" s="121"/>
+      <c r="V16" s="121"/>
+      <c r="W16" s="121"/>
+      <c r="X16" s="121"/>
+      <c r="Y16" s="121"/>
+      <c r="Z16" s="121"/>
+      <c r="AA16" s="121"/>
+      <c r="AB16" s="121"/>
+      <c r="AC16" s="121"/>
+      <c r="AD16" s="121"/>
+      <c r="AE16" s="121"/>
+      <c r="AF16" s="121"/>
+      <c r="AG16" s="121"/>
+      <c r="AH16" s="121"/>
+      <c r="AI16" s="121"/>
+      <c r="AJ16" s="121"/>
+      <c r="AK16" s="121"/>
+      <c r="AL16" s="121"/>
+      <c r="AM16" s="121"/>
+      <c r="AN16" s="121"/>
+      <c r="AO16" s="121"/>
+      <c r="AP16" s="121"/>
+      <c r="AQ16" s="121"/>
+      <c r="AR16" s="121"/>
+      <c r="AS16" s="121"/>
+      <c r="AT16" s="121"/>
+      <c r="AU16" s="121"/>
+      <c r="AV16" s="121"/>
+      <c r="AW16" s="121"/>
+      <c r="AX16" s="121"/>
+      <c r="AY16" s="121"/>
+      <c r="AZ16" s="121"/>
+      <c r="BA16" s="121"/>
+      <c r="BB16" s="121"/>
+      <c r="BC16" s="122"/>
     </row>
     <row r="17" spans="2:55">
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="123" t="s">
         <v>827</v>
       </c>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="102"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
+      <c r="E17" s="124"/>
+      <c r="F17" s="125"/>
       <c r="G17" s="33"/>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
@@ -42011,21 +42014,21 @@
         <v>816</v>
       </c>
       <c r="AY17" s="38"/>
-      <c r="AZ17" s="115" t="s">
+      <c r="AZ17" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="BA17" s="115"/>
-      <c r="BB17" s="115"/>
+      <c r="BA17" s="66"/>
+      <c r="BB17" s="66"/>
       <c r="BC17" s="39"/>
     </row>
     <row r="18" spans="2:55">
-      <c r="B18" s="103" t="s">
+      <c r="B18" s="100" t="s">
         <v>828</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="105"/>
+      <c r="C18" s="101"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="102"/>
       <c r="G18" s="6"/>
       <c r="L18" s="6"/>
       <c r="R18" s="6"/>
@@ -42034,24 +42037,24 @@
       <c r="AJ18" s="6"/>
       <c r="AP18" s="6"/>
       <c r="AV18" s="6"/>
-      <c r="AX18" s="84" t="e">
+      <c r="AX18" s="67" t="e">
         <f>INDEX(TblCardDesign[#Data],MATCH(AY17,TblCardDesign[ID],0),3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AY18" s="85"/>
-      <c r="AZ18" s="85"/>
-      <c r="BA18" s="85"/>
-      <c r="BB18" s="85"/>
+      <c r="AY18" s="68"/>
+      <c r="AZ18" s="68"/>
+      <c r="BA18" s="68"/>
+      <c r="BB18" s="68"/>
       <c r="BC18" s="40"/>
     </row>
     <row r="19" spans="2:55">
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="103" t="s">
         <v>829</v>
       </c>
-      <c r="C19" s="107"/>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="108"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="105"/>
       <c r="G19" s="35"/>
       <c r="L19" s="35"/>
       <c r="R19" s="35"/>
@@ -42060,24 +42063,24 @@
       <c r="AJ19" s="35"/>
       <c r="AP19" s="35"/>
       <c r="AV19" s="35"/>
-      <c r="AX19" s="82" t="e">
+      <c r="AX19" s="69" t="e">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AY17,TblCardDesign[ID],0),11)</f>
         <v>#N/A</v>
       </c>
-      <c r="AY19" s="83"/>
-      <c r="AZ19" s="83"/>
-      <c r="BA19" s="83"/>
-      <c r="BB19" s="83"/>
+      <c r="AY19" s="70"/>
+      <c r="AZ19" s="70"/>
+      <c r="BA19" s="70"/>
+      <c r="BB19" s="70"/>
       <c r="BC19" s="41"/>
     </row>
     <row r="20" spans="2:55" ht="15.75" thickBot="1">
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="126" t="s">
         <v>830</v>
       </c>
-      <c r="C20" s="110"/>
-      <c r="D20" s="110"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="111"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="128"/>
       <c r="G20" s="6"/>
       <c r="L20" s="6"/>
       <c r="R20" s="6"/>
@@ -42134,67 +42137,67 @@
     </row>
     <row r="22" spans="2:55">
       <c r="B22" s="7"/>
-      <c r="AX22" s="84" t="s">
+      <c r="AX22" s="67" t="s">
         <v>824</v>
       </c>
-      <c r="AY22" s="85"/>
-      <c r="AZ22" s="85"/>
-      <c r="BA22" s="85"/>
-      <c r="BB22" s="85"/>
+      <c r="AY22" s="68"/>
+      <c r="AZ22" s="68"/>
+      <c r="BA22" s="68"/>
+      <c r="BB22" s="68"/>
       <c r="BC22" s="40"/>
     </row>
     <row r="23" spans="2:55">
       <c r="B23" s="7"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
-      <c r="M23" s="128"/>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
-      <c r="AX23" s="86" t="e">
+      <c r="K23" s="65"/>
+      <c r="L23" s="65"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="AX23" s="71" t="e">
         <f>INDEX(TblCardDesign[#Data],MATCH(AY17,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>#N/A</v>
       </c>
-      <c r="AY23" s="87"/>
-      <c r="AZ23" s="87"/>
-      <c r="BA23" s="87"/>
-      <c r="BB23" s="87"/>
-      <c r="BC23" s="88"/>
+      <c r="AY23" s="72"/>
+      <c r="AZ23" s="72"/>
+      <c r="BA23" s="72"/>
+      <c r="BB23" s="72"/>
+      <c r="BC23" s="73"/>
     </row>
     <row r="24" spans="2:55">
       <c r="B24" s="7"/>
-      <c r="AX24" s="86"/>
-      <c r="AY24" s="87"/>
-      <c r="AZ24" s="87"/>
-      <c r="BA24" s="87"/>
-      <c r="BB24" s="87"/>
-      <c r="BC24" s="88"/>
+      <c r="AX24" s="71"/>
+      <c r="AY24" s="72"/>
+      <c r="AZ24" s="72"/>
+      <c r="BA24" s="72"/>
+      <c r="BB24" s="72"/>
+      <c r="BC24" s="73"/>
     </row>
     <row r="25" spans="2:55">
       <c r="B25" s="7"/>
-      <c r="AX25" s="86"/>
-      <c r="AY25" s="87"/>
-      <c r="AZ25" s="87"/>
-      <c r="BA25" s="87"/>
-      <c r="BB25" s="87"/>
-      <c r="BC25" s="88"/>
+      <c r="AX25" s="71"/>
+      <c r="AY25" s="72"/>
+      <c r="AZ25" s="72"/>
+      <c r="BA25" s="72"/>
+      <c r="BB25" s="72"/>
+      <c r="BC25" s="73"/>
     </row>
     <row r="26" spans="2:55">
       <c r="B26" s="7"/>
-      <c r="AX26" s="86"/>
-      <c r="AY26" s="87"/>
-      <c r="AZ26" s="87"/>
-      <c r="BA26" s="87"/>
-      <c r="BB26" s="87"/>
-      <c r="BC26" s="88"/>
+      <c r="AX26" s="71"/>
+      <c r="AY26" s="72"/>
+      <c r="AZ26" s="72"/>
+      <c r="BA26" s="72"/>
+      <c r="BB26" s="72"/>
+      <c r="BC26" s="73"/>
     </row>
     <row r="27" spans="2:55" ht="15.75" thickBot="1">
       <c r="B27" s="7"/>
-      <c r="AX27" s="89"/>
-      <c r="AY27" s="90"/>
-      <c r="AZ27" s="90"/>
-      <c r="BA27" s="90"/>
-      <c r="BB27" s="90"/>
-      <c r="BC27" s="91"/>
+      <c r="AX27" s="74"/>
+      <c r="AY27" s="75"/>
+      <c r="AZ27" s="75"/>
+      <c r="BA27" s="75"/>
+      <c r="BB27" s="75"/>
+      <c r="BC27" s="76"/>
     </row>
     <row r="28" spans="2:55" ht="15.75" thickBot="1">
       <c r="B28" s="46" t="s">
@@ -42247,49 +42250,49 @@
       <c r="AU28" s="36"/>
       <c r="AV28" s="36"/>
       <c r="AW28" s="36"/>
-      <c r="AX28" s="92" t="s">
+      <c r="AX28" s="117" t="s">
         <v>831</v>
       </c>
-      <c r="AY28" s="93"/>
-      <c r="AZ28" s="93"/>
-      <c r="BA28" s="93"/>
-      <c r="BB28" s="93"/>
-      <c r="BC28" s="94"/>
+      <c r="AY28" s="118"/>
+      <c r="AZ28" s="118"/>
+      <c r="BA28" s="118"/>
+      <c r="BB28" s="118"/>
+      <c r="BC28" s="119"/>
     </row>
     <row r="29" spans="2:55">
       <c r="B29" s="37" t="s">
         <v>816</v>
       </c>
       <c r="C29" s="38"/>
-      <c r="D29" s="115" t="s">
+      <c r="D29" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="115"/>
-      <c r="F29" s="115"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
       <c r="G29" s="39"/>
       <c r="BC29" s="8"/>
     </row>
     <row r="30" spans="2:55">
-      <c r="B30" s="84" t="e">
+      <c r="B30" s="67" t="e">
         <f>INDEX(TblCardDesign[#Data],MATCH(C29,TblCardDesign[ID],0),3)</f>
         <v>#N/A</v>
       </c>
-      <c r="C30" s="85"/>
-      <c r="D30" s="85"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
       <c r="G30" s="40"/>
       <c r="BC30" s="8"/>
     </row>
     <row r="31" spans="2:55">
-      <c r="B31" s="82" t="e">
+      <c r="B31" s="69" t="e">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(C29,TblCardDesign[ID],0),11)</f>
         <v>#N/A</v>
       </c>
-      <c r="C31" s="83"/>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="41"/>
       <c r="BC31" s="8"/>
     </row>
@@ -42342,83 +42345,83 @@
       <c r="BC33" s="8"/>
     </row>
     <row r="34" spans="2:55">
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="67" t="s">
         <v>824</v>
       </c>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
       <c r="G34" s="40"/>
       <c r="BC34" s="8"/>
     </row>
     <row r="35" spans="2:55" ht="15.75" thickBot="1">
-      <c r="B35" s="86" t="e">
+      <c r="B35" s="71" t="e">
         <f>INDEX(TblCardDesign[#Data],MATCH(C29,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>#N/A</v>
       </c>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="88"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
       <c r="BC35" s="8"/>
     </row>
     <row r="36" spans="2:55">
-      <c r="B36" s="86"/>
-      <c r="C36" s="87"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="88"/>
-      <c r="AX36" s="122" t="s">
+      <c r="B36" s="71"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
+      <c r="AX36" s="106" t="s">
         <v>830</v>
       </c>
-      <c r="AY36" s="123"/>
-      <c r="AZ36" s="123"/>
-      <c r="BA36" s="123"/>
-      <c r="BB36" s="123"/>
-      <c r="BC36" s="124"/>
+      <c r="AY36" s="107"/>
+      <c r="AZ36" s="107"/>
+      <c r="BA36" s="107"/>
+      <c r="BB36" s="107"/>
+      <c r="BC36" s="108"/>
     </row>
     <row r="37" spans="2:55">
-      <c r="B37" s="86"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="88"/>
-      <c r="AX37" s="106" t="s">
+      <c r="B37" s="71"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="73"/>
+      <c r="AX37" s="103" t="s">
         <v>829</v>
       </c>
-      <c r="AY37" s="107"/>
-      <c r="AZ37" s="107"/>
-      <c r="BA37" s="107"/>
-      <c r="BB37" s="107"/>
-      <c r="BC37" s="108"/>
+      <c r="AY37" s="104"/>
+      <c r="AZ37" s="104"/>
+      <c r="BA37" s="104"/>
+      <c r="BB37" s="104"/>
+      <c r="BC37" s="105"/>
     </row>
     <row r="38" spans="2:55">
-      <c r="B38" s="86"/>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="88"/>
-      <c r="AX38" s="103" t="s">
+      <c r="B38" s="71"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="73"/>
+      <c r="AX38" s="100" t="s">
         <v>828</v>
       </c>
-      <c r="AY38" s="104"/>
-      <c r="AZ38" s="104"/>
-      <c r="BA38" s="104"/>
-      <c r="BB38" s="104"/>
-      <c r="BC38" s="105"/>
+      <c r="AY38" s="101"/>
+      <c r="AZ38" s="101"/>
+      <c r="BA38" s="101"/>
+      <c r="BB38" s="101"/>
+      <c r="BC38" s="102"/>
     </row>
     <row r="39" spans="2:55" ht="15.75" thickBot="1">
-      <c r="B39" s="89"/>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="90"/>
-      <c r="F39" s="90"/>
-      <c r="G39" s="91"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="75"/>
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="76"/>
       <c r="H39" s="18"/>
       <c r="I39" s="18"/>
       <c r="J39" s="18"/>
@@ -42461,206 +42464,206 @@
       <c r="AU39" s="18"/>
       <c r="AV39" s="18"/>
       <c r="AW39" s="18"/>
-      <c r="AX39" s="119" t="s">
+      <c r="AX39" s="97" t="s">
         <v>827</v>
       </c>
-      <c r="AY39" s="120"/>
-      <c r="AZ39" s="120"/>
-      <c r="BA39" s="120"/>
-      <c r="BB39" s="120"/>
-      <c r="BC39" s="121"/>
+      <c r="AY39" s="98"/>
+      <c r="AZ39" s="98"/>
+      <c r="BA39" s="98"/>
+      <c r="BB39" s="98"/>
+      <c r="BC39" s="99"/>
     </row>
     <row r="40" spans="2:55" ht="16.5" thickBot="1">
-      <c r="B40" s="116" t="s">
+      <c r="B40" s="94" t="s">
         <v>832</v>
       </c>
-      <c r="C40" s="117"/>
-      <c r="D40" s="117"/>
-      <c r="E40" s="117"/>
-      <c r="F40" s="117"/>
-      <c r="G40" s="117"/>
-      <c r="H40" s="117"/>
-      <c r="I40" s="117"/>
-      <c r="J40" s="117"/>
-      <c r="K40" s="117"/>
-      <c r="L40" s="117"/>
-      <c r="M40" s="117"/>
-      <c r="N40" s="117"/>
-      <c r="O40" s="117"/>
-      <c r="P40" s="117"/>
-      <c r="Q40" s="117"/>
-      <c r="R40" s="117"/>
-      <c r="S40" s="117"/>
-      <c r="T40" s="117"/>
-      <c r="U40" s="117"/>
-      <c r="V40" s="117"/>
-      <c r="W40" s="117"/>
-      <c r="X40" s="117"/>
-      <c r="Y40" s="117"/>
-      <c r="Z40" s="117"/>
-      <c r="AA40" s="117"/>
-      <c r="AB40" s="117"/>
-      <c r="AC40" s="117"/>
-      <c r="AD40" s="117"/>
-      <c r="AE40" s="117"/>
-      <c r="AF40" s="117"/>
-      <c r="AG40" s="117"/>
-      <c r="AH40" s="117"/>
-      <c r="AI40" s="117"/>
-      <c r="AJ40" s="117"/>
-      <c r="AK40" s="117"/>
-      <c r="AL40" s="117"/>
-      <c r="AM40" s="117"/>
-      <c r="AN40" s="117"/>
-      <c r="AO40" s="117"/>
-      <c r="AP40" s="117"/>
-      <c r="AQ40" s="117"/>
-      <c r="AR40" s="117"/>
-      <c r="AS40" s="117"/>
-      <c r="AT40" s="117"/>
-      <c r="AU40" s="117"/>
-      <c r="AV40" s="117"/>
-      <c r="AW40" s="117"/>
-      <c r="AX40" s="117"/>
-      <c r="AY40" s="117"/>
-      <c r="AZ40" s="117"/>
-      <c r="BA40" s="117"/>
-      <c r="BB40" s="117"/>
-      <c r="BC40" s="118"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="95"/>
+      <c r="I40" s="95"/>
+      <c r="J40" s="95"/>
+      <c r="K40" s="95"/>
+      <c r="L40" s="95"/>
+      <c r="M40" s="95"/>
+      <c r="N40" s="95"/>
+      <c r="O40" s="95"/>
+      <c r="P40" s="95"/>
+      <c r="Q40" s="95"/>
+      <c r="R40" s="95"/>
+      <c r="S40" s="95"/>
+      <c r="T40" s="95"/>
+      <c r="U40" s="95"/>
+      <c r="V40" s="95"/>
+      <c r="W40" s="95"/>
+      <c r="X40" s="95"/>
+      <c r="Y40" s="95"/>
+      <c r="Z40" s="95"/>
+      <c r="AA40" s="95"/>
+      <c r="AB40" s="95"/>
+      <c r="AC40" s="95"/>
+      <c r="AD40" s="95"/>
+      <c r="AE40" s="95"/>
+      <c r="AF40" s="95"/>
+      <c r="AG40" s="95"/>
+      <c r="AH40" s="95"/>
+      <c r="AI40" s="95"/>
+      <c r="AJ40" s="95"/>
+      <c r="AK40" s="95"/>
+      <c r="AL40" s="95"/>
+      <c r="AM40" s="95"/>
+      <c r="AN40" s="95"/>
+      <c r="AO40" s="95"/>
+      <c r="AP40" s="95"/>
+      <c r="AQ40" s="95"/>
+      <c r="AR40" s="95"/>
+      <c r="AS40" s="95"/>
+      <c r="AT40" s="95"/>
+      <c r="AU40" s="95"/>
+      <c r="AV40" s="95"/>
+      <c r="AW40" s="95"/>
+      <c r="AX40" s="95"/>
+      <c r="AY40" s="95"/>
+      <c r="AZ40" s="95"/>
+      <c r="BA40" s="95"/>
+      <c r="BB40" s="95"/>
+      <c r="BC40" s="96"/>
     </row>
     <row r="41" spans="2:55" ht="15.75" thickBot="1">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="83" t="s">
         <v>804</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="70"/>
-      <c r="M41" s="70"/>
-      <c r="N41" s="70"/>
-      <c r="O41" s="70"/>
-      <c r="P41" s="70"/>
-      <c r="Q41" s="70"/>
-      <c r="R41" s="70"/>
-      <c r="S41" s="70"/>
-      <c r="T41" s="70"/>
-      <c r="U41" s="70"/>
-      <c r="V41" s="70"/>
-      <c r="W41" s="70"/>
-      <c r="X41" s="70"/>
-      <c r="Y41" s="70"/>
-      <c r="Z41" s="70"/>
-      <c r="AA41" s="70"/>
-      <c r="AB41" s="70"/>
-      <c r="AC41" s="70"/>
-      <c r="AD41" s="70"/>
-      <c r="AE41" s="70"/>
-      <c r="AF41" s="70"/>
-      <c r="AG41" s="70"/>
-      <c r="AH41" s="70"/>
-      <c r="AI41" s="70"/>
-      <c r="AJ41" s="70"/>
-      <c r="AK41" s="71"/>
-      <c r="AL41" s="69" t="s">
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="84"/>
+      <c r="L41" s="84"/>
+      <c r="M41" s="84"/>
+      <c r="N41" s="84"/>
+      <c r="O41" s="84"/>
+      <c r="P41" s="84"/>
+      <c r="Q41" s="84"/>
+      <c r="R41" s="84"/>
+      <c r="S41" s="84"/>
+      <c r="T41" s="84"/>
+      <c r="U41" s="84"/>
+      <c r="V41" s="84"/>
+      <c r="W41" s="84"/>
+      <c r="X41" s="84"/>
+      <c r="Y41" s="84"/>
+      <c r="Z41" s="84"/>
+      <c r="AA41" s="84"/>
+      <c r="AB41" s="84"/>
+      <c r="AC41" s="84"/>
+      <c r="AD41" s="84"/>
+      <c r="AE41" s="84"/>
+      <c r="AF41" s="84"/>
+      <c r="AG41" s="84"/>
+      <c r="AH41" s="84"/>
+      <c r="AI41" s="84"/>
+      <c r="AJ41" s="84"/>
+      <c r="AK41" s="85"/>
+      <c r="AL41" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="AM41" s="70"/>
-      <c r="AN41" s="70"/>
-      <c r="AO41" s="70"/>
-      <c r="AP41" s="70"/>
-      <c r="AQ41" s="70"/>
-      <c r="AR41" s="70"/>
-      <c r="AS41" s="70"/>
-      <c r="AT41" s="70"/>
-      <c r="AU41" s="70"/>
-      <c r="AV41" s="70"/>
-      <c r="AW41" s="70"/>
-      <c r="AX41" s="70"/>
-      <c r="AY41" s="70"/>
-      <c r="AZ41" s="70"/>
-      <c r="BA41" s="70"/>
-      <c r="BB41" s="70"/>
-      <c r="BC41" s="71"/>
+      <c r="AM41" s="84"/>
+      <c r="AN41" s="84"/>
+      <c r="AO41" s="84"/>
+      <c r="AP41" s="84"/>
+      <c r="AQ41" s="84"/>
+      <c r="AR41" s="84"/>
+      <c r="AS41" s="84"/>
+      <c r="AT41" s="84"/>
+      <c r="AU41" s="84"/>
+      <c r="AV41" s="84"/>
+      <c r="AW41" s="84"/>
+      <c r="AX41" s="84"/>
+      <c r="AY41" s="84"/>
+      <c r="AZ41" s="84"/>
+      <c r="BA41" s="84"/>
+      <c r="BB41" s="84"/>
+      <c r="BC41" s="85"/>
     </row>
     <row r="42" spans="2:55" ht="15.75" thickBot="1">
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="78" t="s">
         <v>805</v>
       </c>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="79"/>
       <c r="G42" s="27"/>
-      <c r="H42" s="77" t="s">
+      <c r="H42" s="80" t="s">
         <v>806</v>
       </c>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="76"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="78"/>
-      <c r="N42" s="76" t="s">
+      <c r="I42" s="79"/>
+      <c r="J42" s="79"/>
+      <c r="K42" s="79"/>
+      <c r="L42" s="79"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="79" t="s">
         <v>807</v>
       </c>
-      <c r="O42" s="76"/>
-      <c r="P42" s="76"/>
-      <c r="Q42" s="76"/>
-      <c r="R42" s="76"/>
-      <c r="S42" s="76"/>
-      <c r="T42" s="77" t="s">
+      <c r="O42" s="79"/>
+      <c r="P42" s="79"/>
+      <c r="Q42" s="79"/>
+      <c r="R42" s="79"/>
+      <c r="S42" s="79"/>
+      <c r="T42" s="80" t="s">
         <v>808</v>
       </c>
-      <c r="U42" s="76"/>
-      <c r="V42" s="76"/>
-      <c r="W42" s="76"/>
-      <c r="X42" s="76"/>
-      <c r="Y42" s="78"/>
-      <c r="Z42" s="76" t="s">
+      <c r="U42" s="79"/>
+      <c r="V42" s="79"/>
+      <c r="W42" s="79"/>
+      <c r="X42" s="79"/>
+      <c r="Y42" s="81"/>
+      <c r="Z42" s="79" t="s">
         <v>809</v>
       </c>
-      <c r="AA42" s="76"/>
-      <c r="AB42" s="76"/>
-      <c r="AC42" s="76"/>
-      <c r="AD42" s="76"/>
-      <c r="AE42" s="76"/>
-      <c r="AF42" s="77" t="s">
+      <c r="AA42" s="79"/>
+      <c r="AB42" s="79"/>
+      <c r="AC42" s="79"/>
+      <c r="AD42" s="79"/>
+      <c r="AE42" s="79"/>
+      <c r="AF42" s="80" t="s">
         <v>810</v>
       </c>
-      <c r="AG42" s="76"/>
-      <c r="AH42" s="76"/>
-      <c r="AI42" s="76"/>
-      <c r="AJ42" s="76"/>
-      <c r="AK42" s="76"/>
-      <c r="AL42" s="75" t="s">
+      <c r="AG42" s="79"/>
+      <c r="AH42" s="79"/>
+      <c r="AI42" s="79"/>
+      <c r="AJ42" s="79"/>
+      <c r="AK42" s="79"/>
+      <c r="AL42" s="78" t="s">
         <v>811</v>
       </c>
-      <c r="AM42" s="76"/>
-      <c r="AN42" s="76"/>
-      <c r="AO42" s="76"/>
-      <c r="AP42" s="76"/>
-      <c r="AQ42" s="76"/>
-      <c r="AR42" s="77" t="s">
+      <c r="AM42" s="79"/>
+      <c r="AN42" s="79"/>
+      <c r="AO42" s="79"/>
+      <c r="AP42" s="79"/>
+      <c r="AQ42" s="79"/>
+      <c r="AR42" s="80" t="s">
         <v>812</v>
       </c>
-      <c r="AS42" s="76"/>
-      <c r="AT42" s="76"/>
-      <c r="AU42" s="76"/>
-      <c r="AV42" s="76"/>
-      <c r="AW42" s="78"/>
-      <c r="AX42" s="76" t="s">
+      <c r="AS42" s="79"/>
+      <c r="AT42" s="79"/>
+      <c r="AU42" s="79"/>
+      <c r="AV42" s="79"/>
+      <c r="AW42" s="81"/>
+      <c r="AX42" s="79" t="s">
         <v>813</v>
       </c>
-      <c r="AY42" s="76"/>
-      <c r="AZ42" s="76"/>
-      <c r="BA42" s="76"/>
-      <c r="BB42" s="76"/>
-      <c r="BC42" s="127"/>
+      <c r="AY42" s="79"/>
+      <c r="AZ42" s="79"/>
+      <c r="BA42" s="79"/>
+      <c r="BB42" s="79"/>
+      <c r="BC42" s="82"/>
     </row>
     <row r="43" spans="2:55">
       <c r="B43" s="9" t="s">
@@ -42669,12 +42672,12 @@
       <c r="C43" s="26">
         <v>63</v>
       </c>
-      <c r="D43" s="72" t="str">
+      <c r="D43" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(C43,TblCardDesign[ID],0),14)</f>
         <v>Rank: 2</v>
       </c>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
       <c r="G43" s="10"/>
       <c r="H43" s="31" t="s">
         <v>816</v>
@@ -42682,270 +42685,270 @@
       <c r="I43" s="32">
         <v>99</v>
       </c>
-      <c r="J43" s="95" t="str">
+      <c r="J43" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(I43,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="K43" s="95"/>
-      <c r="L43" s="95"/>
-      <c r="M43" s="96"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="64"/>
       <c r="N43" s="10" t="s">
         <v>816</v>
       </c>
       <c r="O43" s="26">
         <v>46</v>
       </c>
-      <c r="P43" s="72" t="str">
+      <c r="P43" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(O43,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="Q43" s="72"/>
-      <c r="R43" s="72"/>
-      <c r="S43" s="72"/>
+      <c r="Q43" s="77"/>
+      <c r="R43" s="77"/>
+      <c r="S43" s="77"/>
       <c r="T43" s="31" t="s">
         <v>816</v>
       </c>
       <c r="U43" s="32">
         <v>56</v>
       </c>
-      <c r="V43" s="95" t="str">
+      <c r="V43" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(U43,TblCardDesign[ID],0),14)</f>
         <v>Rank: 1</v>
       </c>
-      <c r="W43" s="95"/>
-      <c r="X43" s="95"/>
-      <c r="Y43" s="96"/>
+      <c r="W43" s="63"/>
+      <c r="X43" s="63"/>
+      <c r="Y43" s="64"/>
       <c r="Z43" s="10" t="s">
         <v>816</v>
       </c>
       <c r="AA43" s="26">
         <v>99</v>
       </c>
-      <c r="AB43" s="72" t="str">
+      <c r="AB43" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AA43,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="AC43" s="72"/>
-      <c r="AD43" s="72"/>
-      <c r="AE43" s="72"/>
+      <c r="AC43" s="77"/>
+      <c r="AD43" s="77"/>
+      <c r="AE43" s="77"/>
       <c r="AF43" s="31" t="s">
         <v>816</v>
       </c>
       <c r="AG43" s="32">
         <v>62</v>
       </c>
-      <c r="AH43" s="95" t="str">
+      <c r="AH43" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AG43,TblCardDesign[ID],0),14)</f>
         <v>Rank: 2</v>
       </c>
-      <c r="AI43" s="95"/>
-      <c r="AJ43" s="95"/>
-      <c r="AK43" s="96"/>
+      <c r="AI43" s="63"/>
+      <c r="AJ43" s="63"/>
+      <c r="AK43" s="64"/>
       <c r="AL43" s="10" t="s">
         <v>816</v>
       </c>
       <c r="AM43" s="26">
         <v>82</v>
       </c>
-      <c r="AN43" s="72" t="str">
+      <c r="AN43" s="77" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AM43,TblCardDesign[ID],0),14)</f>
         <v xml:space="preserve">Rank: </v>
       </c>
-      <c r="AO43" s="72"/>
-      <c r="AP43" s="72"/>
-      <c r="AQ43" s="72"/>
+      <c r="AO43" s="77"/>
+      <c r="AP43" s="77"/>
+      <c r="AQ43" s="77"/>
       <c r="AR43" s="31" t="s">
         <v>816</v>
       </c>
       <c r="AS43" s="32">
         <v>11</v>
       </c>
-      <c r="AT43" s="95" t="str">
+      <c r="AT43" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AS43,TblCardDesign[ID],0),14)</f>
         <v>Rank: 3</v>
       </c>
-      <c r="AU43" s="95"/>
-      <c r="AV43" s="95"/>
-      <c r="AW43" s="96"/>
+      <c r="AU43" s="63"/>
+      <c r="AV43" s="63"/>
+      <c r="AW43" s="64"/>
       <c r="AX43" s="31" t="s">
         <v>816</v>
       </c>
       <c r="AY43" s="32">
         <v>4</v>
       </c>
-      <c r="AZ43" s="95" t="str">
+      <c r="AZ43" s="63" t="str">
         <f>"Rank: "&amp;INDEX(TblCardDesign[#Data],MATCH(AY43,TblCardDesign[ID],0),14)</f>
         <v>Rank: 1</v>
       </c>
-      <c r="BA43" s="95"/>
-      <c r="BB43" s="95"/>
-      <c r="BC43" s="96"/>
+      <c r="BA43" s="63"/>
+      <c r="BB43" s="63"/>
+      <c r="BC43" s="64"/>
     </row>
     <row r="44" spans="2:55">
-      <c r="B44" s="73" t="str">
+      <c r="B44" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(C43,TblCardDesign[ID],0),3)</f>
         <v>P Bot Bot</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="73" t="str">
+      <c r="H44" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(I43,TblCardDesign[ID],0),3)</f>
         <v>Auto Cannon</v>
       </c>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="72"/>
-      <c r="L44" s="72"/>
-      <c r="M44" s="74"/>
-      <c r="N44" s="72" t="str">
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
+      <c r="M44" s="113"/>
+      <c r="N44" s="77" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(O43,TblCardDesign[ID],0),3)</f>
         <v>Hull Breach</v>
       </c>
-      <c r="O44" s="72"/>
-      <c r="P44" s="72"/>
-      <c r="Q44" s="72"/>
-      <c r="R44" s="72"/>
-      <c r="S44" s="72"/>
-      <c r="T44" s="73" t="str">
+      <c r="O44" s="77"/>
+      <c r="P44" s="77"/>
+      <c r="Q44" s="77"/>
+      <c r="R44" s="77"/>
+      <c r="S44" s="77"/>
+      <c r="T44" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(U43,TblCardDesign[ID],0),3)</f>
         <v>R Bot</v>
       </c>
-      <c r="U44" s="72"/>
-      <c r="V44" s="72"/>
-      <c r="W44" s="72"/>
-      <c r="X44" s="72"/>
-      <c r="Y44" s="74"/>
-      <c r="Z44" s="72" t="str">
+      <c r="U44" s="77"/>
+      <c r="V44" s="77"/>
+      <c r="W44" s="77"/>
+      <c r="X44" s="77"/>
+      <c r="Y44" s="113"/>
+      <c r="Z44" s="77" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AA43,TblCardDesign[ID],0),3)</f>
         <v>Auto Cannon</v>
       </c>
-      <c r="AA44" s="72"/>
-      <c r="AB44" s="72"/>
-      <c r="AC44" s="72"/>
-      <c r="AD44" s="72"/>
-      <c r="AE44" s="72"/>
-      <c r="AF44" s="73" t="str">
+      <c r="AA44" s="77"/>
+      <c r="AB44" s="77"/>
+      <c r="AC44" s="77"/>
+      <c r="AD44" s="77"/>
+      <c r="AE44" s="77"/>
+      <c r="AF44" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AG43,TblCardDesign[ID],0),3)</f>
         <v>B Bot Bot</v>
       </c>
-      <c r="AG44" s="72"/>
-      <c r="AH44" s="72"/>
-      <c r="AI44" s="72"/>
-      <c r="AJ44" s="72"/>
-      <c r="AK44" s="74"/>
-      <c r="AL44" s="72" t="str">
+      <c r="AG44" s="77"/>
+      <c r="AH44" s="77"/>
+      <c r="AI44" s="77"/>
+      <c r="AJ44" s="77"/>
+      <c r="AK44" s="113"/>
+      <c r="AL44" s="77" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AM43,TblCardDesign[ID],0),3)</f>
         <v>Adm. I.T.S Atrap</v>
       </c>
-      <c r="AM44" s="72"/>
-      <c r="AN44" s="72"/>
-      <c r="AO44" s="72"/>
-      <c r="AP44" s="72"/>
-      <c r="AQ44" s="72"/>
-      <c r="AR44" s="73" t="str">
+      <c r="AM44" s="77"/>
+      <c r="AN44" s="77"/>
+      <c r="AO44" s="77"/>
+      <c r="AP44" s="77"/>
+      <c r="AQ44" s="77"/>
+      <c r="AR44" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AS43,TblCardDesign[ID],0),3)</f>
         <v>Chief Medical Officer</v>
       </c>
-      <c r="AS44" s="72"/>
-      <c r="AT44" s="72"/>
-      <c r="AU44" s="72"/>
-      <c r="AV44" s="72"/>
-      <c r="AW44" s="74"/>
-      <c r="AX44" s="73" t="str">
+      <c r="AS44" s="77"/>
+      <c r="AT44" s="77"/>
+      <c r="AU44" s="77"/>
+      <c r="AV44" s="77"/>
+      <c r="AW44" s="113"/>
+      <c r="AX44" s="112" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AY43,TblCardDesign[ID],0),3)</f>
         <v>Mad Scientist</v>
       </c>
-      <c r="AY44" s="72"/>
-      <c r="AZ44" s="72"/>
-      <c r="BA44" s="72"/>
-      <c r="BB44" s="72"/>
-      <c r="BC44" s="74"/>
+      <c r="AY44" s="77"/>
+      <c r="AZ44" s="77"/>
+      <c r="BA44" s="77"/>
+      <c r="BB44" s="77"/>
+      <c r="BC44" s="113"/>
     </row>
     <row r="45" spans="2:55">
-      <c r="B45" s="112" t="str">
+      <c r="B45" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(C43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="C45" s="113"/>
-      <c r="D45" s="113"/>
-      <c r="E45" s="113"/>
-      <c r="F45" s="113"/>
+      <c r="C45" s="115"/>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="115"/>
       <c r="G45" s="11"/>
-      <c r="H45" s="112" t="str">
+      <c r="H45" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(I43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="I45" s="113"/>
-      <c r="J45" s="113"/>
-      <c r="K45" s="113"/>
-      <c r="L45" s="113"/>
-      <c r="M45" s="114"/>
-      <c r="N45" s="113" t="str">
+      <c r="I45" s="115"/>
+      <c r="J45" s="115"/>
+      <c r="K45" s="115"/>
+      <c r="L45" s="115"/>
+      <c r="M45" s="116"/>
+      <c r="N45" s="115" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(O43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="O45" s="113"/>
-      <c r="P45" s="113"/>
-      <c r="Q45" s="113"/>
-      <c r="R45" s="113"/>
-      <c r="S45" s="113"/>
-      <c r="T45" s="112" t="str">
+      <c r="O45" s="115"/>
+      <c r="P45" s="115"/>
+      <c r="Q45" s="115"/>
+      <c r="R45" s="115"/>
+      <c r="S45" s="115"/>
+      <c r="T45" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(U43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="U45" s="113"/>
-      <c r="V45" s="113"/>
-      <c r="W45" s="113"/>
-      <c r="X45" s="113"/>
-      <c r="Y45" s="114"/>
-      <c r="Z45" s="113" t="str">
+      <c r="U45" s="115"/>
+      <c r="V45" s="115"/>
+      <c r="W45" s="115"/>
+      <c r="X45" s="115"/>
+      <c r="Y45" s="116"/>
+      <c r="Z45" s="115" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AA43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AA45" s="113"/>
-      <c r="AB45" s="113"/>
-      <c r="AC45" s="113"/>
-      <c r="AD45" s="113"/>
-      <c r="AE45" s="113"/>
-      <c r="AF45" s="112" t="str">
+      <c r="AA45" s="115"/>
+      <c r="AB45" s="115"/>
+      <c r="AC45" s="115"/>
+      <c r="AD45" s="115"/>
+      <c r="AE45" s="115"/>
+      <c r="AF45" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AG43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AG45" s="113"/>
-      <c r="AH45" s="113"/>
-      <c r="AI45" s="113"/>
-      <c r="AJ45" s="113"/>
-      <c r="AK45" s="114"/>
-      <c r="AL45" s="113" t="str">
+      <c r="AG45" s="115"/>
+      <c r="AH45" s="115"/>
+      <c r="AI45" s="115"/>
+      <c r="AJ45" s="115"/>
+      <c r="AK45" s="116"/>
+      <c r="AL45" s="115" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AM43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AM45" s="113"/>
-      <c r="AN45" s="113"/>
-      <c r="AO45" s="113"/>
-      <c r="AP45" s="113"/>
-      <c r="AQ45" s="113"/>
-      <c r="AR45" s="112" t="str">
+      <c r="AM45" s="115"/>
+      <c r="AN45" s="115"/>
+      <c r="AO45" s="115"/>
+      <c r="AP45" s="115"/>
+      <c r="AQ45" s="115"/>
+      <c r="AR45" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AS43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AS45" s="113"/>
-      <c r="AT45" s="113"/>
-      <c r="AU45" s="113"/>
-      <c r="AV45" s="113"/>
-      <c r="AW45" s="114"/>
-      <c r="AX45" s="112" t="str">
+      <c r="AS45" s="115"/>
+      <c r="AT45" s="115"/>
+      <c r="AU45" s="115"/>
+      <c r="AV45" s="115"/>
+      <c r="AW45" s="116"/>
+      <c r="AX45" s="114" t="str">
         <f>"Type: "&amp;INDEX(TblCardDesign[#Data],MATCH(AY43,TblCardDesign[ID],0),11)</f>
         <v xml:space="preserve">Type: </v>
       </c>
-      <c r="AY45" s="113"/>
-      <c r="AZ45" s="113"/>
-      <c r="BA45" s="113"/>
-      <c r="BB45" s="113"/>
-      <c r="BC45" s="114"/>
+      <c r="AY45" s="115"/>
+      <c r="AZ45" s="115"/>
+      <c r="BA45" s="115"/>
+      <c r="BB45" s="115"/>
+      <c r="BC45" s="116"/>
     </row>
     <row r="46" spans="2:55">
       <c r="B46" s="28" t="s">
@@ -43330,509 +43333,620 @@
       </c>
     </row>
     <row r="48" spans="2:55">
-      <c r="B48" s="73" t="s">
+      <c r="B48" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="C48" s="72"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="72"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="77"/>
       <c r="G48" s="10"/>
-      <c r="H48" s="73" t="s">
+      <c r="H48" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="I48" s="72"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="72"/>
-      <c r="L48" s="72"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="72" t="s">
+      <c r="I48" s="77"/>
+      <c r="J48" s="77"/>
+      <c r="K48" s="77"/>
+      <c r="L48" s="77"/>
+      <c r="M48" s="113"/>
+      <c r="N48" s="77" t="s">
         <v>824</v>
       </c>
-      <c r="O48" s="72"/>
-      <c r="P48" s="72"/>
-      <c r="Q48" s="72"/>
-      <c r="R48" s="72"/>
-      <c r="S48" s="72"/>
-      <c r="T48" s="73" t="s">
+      <c r="O48" s="77"/>
+      <c r="P48" s="77"/>
+      <c r="Q48" s="77"/>
+      <c r="R48" s="77"/>
+      <c r="S48" s="77"/>
+      <c r="T48" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="U48" s="72"/>
-      <c r="V48" s="72"/>
-      <c r="W48" s="72"/>
-      <c r="X48" s="72"/>
-      <c r="Y48" s="74"/>
-      <c r="Z48" s="72" t="s">
+      <c r="U48" s="77"/>
+      <c r="V48" s="77"/>
+      <c r="W48" s="77"/>
+      <c r="X48" s="77"/>
+      <c r="Y48" s="113"/>
+      <c r="Z48" s="77" t="s">
         <v>824</v>
       </c>
-      <c r="AA48" s="72"/>
-      <c r="AB48" s="72"/>
-      <c r="AC48" s="72"/>
-      <c r="AD48" s="72"/>
-      <c r="AE48" s="72"/>
-      <c r="AF48" s="73" t="s">
+      <c r="AA48" s="77"/>
+      <c r="AB48" s="77"/>
+      <c r="AC48" s="77"/>
+      <c r="AD48" s="77"/>
+      <c r="AE48" s="77"/>
+      <c r="AF48" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="AG48" s="72"/>
-      <c r="AH48" s="72"/>
-      <c r="AI48" s="72"/>
-      <c r="AJ48" s="72"/>
-      <c r="AK48" s="74"/>
-      <c r="AL48" s="72" t="s">
+      <c r="AG48" s="77"/>
+      <c r="AH48" s="77"/>
+      <c r="AI48" s="77"/>
+      <c r="AJ48" s="77"/>
+      <c r="AK48" s="113"/>
+      <c r="AL48" s="77" t="s">
         <v>824</v>
       </c>
-      <c r="AM48" s="72"/>
-      <c r="AN48" s="72"/>
-      <c r="AO48" s="72"/>
-      <c r="AP48" s="72"/>
-      <c r="AQ48" s="72"/>
-      <c r="AR48" s="79" t="s">
+      <c r="AM48" s="77"/>
+      <c r="AN48" s="77"/>
+      <c r="AO48" s="77"/>
+      <c r="AP48" s="77"/>
+      <c r="AQ48" s="77"/>
+      <c r="AR48" s="109" t="s">
         <v>824</v>
       </c>
-      <c r="AS48" s="80"/>
-      <c r="AT48" s="80"/>
-      <c r="AU48" s="80"/>
-      <c r="AV48" s="80"/>
-      <c r="AW48" s="81"/>
-      <c r="AX48" s="73" t="s">
+      <c r="AS48" s="110"/>
+      <c r="AT48" s="110"/>
+      <c r="AU48" s="110"/>
+      <c r="AV48" s="110"/>
+      <c r="AW48" s="111"/>
+      <c r="AX48" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="AY48" s="72"/>
-      <c r="AZ48" s="72"/>
-      <c r="BA48" s="72"/>
-      <c r="BB48" s="72"/>
-      <c r="BC48" s="74"/>
+      <c r="AY48" s="77"/>
+      <c r="AZ48" s="77"/>
+      <c r="BA48" s="77"/>
+      <c r="BB48" s="77"/>
+      <c r="BC48" s="113"/>
     </row>
     <row r="49" spans="2:55" ht="15" customHeight="1">
-      <c r="B49" s="63" t="str">
+      <c r="B49" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(C43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Sacrifice 1 Assault Tier 1
 Robot can't be used for gun slots.
 Engage: Assault + 2
 Engage: Repair ship by 100</v>
       </c>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="63" t="str">
+      <c r="C49" s="89"/>
+      <c r="D49" s="89"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="89"/>
+      <c r="G49" s="90"/>
+      <c r="H49" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(I43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Attach to Ship: When this ship is targetted by enemy ship gun slots, deal 200 damage to that enemy ship</v>
       </c>
-      <c r="I49" s="64"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="64"/>
-      <c r="M49" s="65"/>
-      <c r="N49" s="64" t="str">
+      <c r="I49" s="89"/>
+      <c r="J49" s="89"/>
+      <c r="K49" s="89"/>
+      <c r="L49" s="89"/>
+      <c r="M49" s="90"/>
+      <c r="N49" s="89" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(O43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Target Enemy Ship: They Sacrifice 1 crew member and take 100 damage to ship</v>
       </c>
-      <c r="O49" s="64"/>
-      <c r="P49" s="64"/>
-      <c r="Q49" s="64"/>
-      <c r="R49" s="64"/>
-      <c r="S49" s="64"/>
-      <c r="T49" s="63" t="str">
+      <c r="O49" s="89"/>
+      <c r="P49" s="89"/>
+      <c r="Q49" s="89"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="89"/>
+      <c r="T49" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(U43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Robot can't be used for gun slots.
 Engage: Medic + 1
 Engage: Repair ship by 100</v>
       </c>
-      <c r="U49" s="64"/>
-      <c r="V49" s="64"/>
-      <c r="W49" s="64"/>
-      <c r="X49" s="64"/>
-      <c r="Y49" s="65"/>
-      <c r="Z49" s="64" t="str">
+      <c r="U49" s="89"/>
+      <c r="V49" s="89"/>
+      <c r="W49" s="89"/>
+      <c r="X49" s="89"/>
+      <c r="Y49" s="90"/>
+      <c r="Z49" s="89" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AA43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Attach to Ship: When this ship is targetted by enemy ship gun slots, deal 200 damage to that enemy ship</v>
       </c>
-      <c r="AA49" s="64"/>
-      <c r="AB49" s="64"/>
-      <c r="AC49" s="64"/>
-      <c r="AD49" s="64"/>
-      <c r="AE49" s="64"/>
-      <c r="AF49" s="63" t="str">
+      <c r="AA49" s="89"/>
+      <c r="AB49" s="89"/>
+      <c r="AC49" s="89"/>
+      <c r="AD49" s="89"/>
+      <c r="AE49" s="89"/>
+      <c r="AF49" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AG43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Sacrifice 1 Handling Tier 1
 Robot can't be used for gun slots.
 Engage: Handling + 2
 Engage: Repair ship by 100</v>
       </c>
-      <c r="AG49" s="64"/>
-      <c r="AH49" s="64"/>
-      <c r="AI49" s="64"/>
-      <c r="AJ49" s="64"/>
-      <c r="AK49" s="65"/>
-      <c r="AL49" s="64" t="str">
+      <c r="AG49" s="89"/>
+      <c r="AH49" s="89"/>
+      <c r="AI49" s="89"/>
+      <c r="AJ49" s="89"/>
+      <c r="AK49" s="90"/>
+      <c r="AL49" s="89" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AM43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Provides 1x Frigate ship when your Capital ship is destroyed, fill crew slots with any crew that wouldve died up to maximum Frigate crew slots.</v>
       </c>
-      <c r="AM49" s="64"/>
-      <c r="AN49" s="64"/>
-      <c r="AO49" s="64"/>
-      <c r="AP49" s="64"/>
-      <c r="AQ49" s="64"/>
-      <c r="AR49" s="63" t="str">
+      <c r="AM49" s="89"/>
+      <c r="AN49" s="89"/>
+      <c r="AO49" s="89"/>
+      <c r="AP49" s="89"/>
+      <c r="AQ49" s="89"/>
+      <c r="AR49" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AS43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Sacrifice 1 Medic Tier 2
 Engage: Medical + 3</v>
       </c>
-      <c r="AS49" s="64"/>
-      <c r="AT49" s="64"/>
-      <c r="AU49" s="64"/>
-      <c r="AV49" s="64"/>
-      <c r="AW49" s="65"/>
-      <c r="AX49" s="63" t="str">
+      <c r="AS49" s="89"/>
+      <c r="AT49" s="89"/>
+      <c r="AU49" s="89"/>
+      <c r="AV49" s="89"/>
+      <c r="AW49" s="90"/>
+      <c r="AX49" s="88" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH(AY43,TblCardDesign[ID],0),'Card Designs'!$Q$3)</f>
         <v>Engage: Discard 1 strategy card from your hand, if you do then Research + 2</v>
       </c>
-      <c r="AY49" s="64"/>
-      <c r="AZ49" s="64"/>
-      <c r="BA49" s="64"/>
-      <c r="BB49" s="64"/>
-      <c r="BC49" s="65"/>
+      <c r="AY49" s="89"/>
+      <c r="AZ49" s="89"/>
+      <c r="BA49" s="89"/>
+      <c r="BB49" s="89"/>
+      <c r="BC49" s="90"/>
     </row>
     <row r="50" spans="2:55">
-      <c r="B50" s="63"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="64"/>
-      <c r="F50" s="64"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="64"/>
-      <c r="J50" s="64"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="64"/>
-      <c r="M50" s="65"/>
-      <c r="N50" s="64"/>
-      <c r="O50" s="64"/>
-      <c r="P50" s="64"/>
-      <c r="Q50" s="64"/>
-      <c r="R50" s="64"/>
-      <c r="S50" s="64"/>
-      <c r="T50" s="63"/>
-      <c r="U50" s="64"/>
-      <c r="V50" s="64"/>
-      <c r="W50" s="64"/>
-      <c r="X50" s="64"/>
-      <c r="Y50" s="65"/>
-      <c r="Z50" s="64"/>
-      <c r="AA50" s="64"/>
-      <c r="AB50" s="64"/>
-      <c r="AC50" s="64"/>
-      <c r="AD50" s="64"/>
-      <c r="AE50" s="64"/>
-      <c r="AF50" s="63"/>
-      <c r="AG50" s="64"/>
-      <c r="AH50" s="64"/>
-      <c r="AI50" s="64"/>
-      <c r="AJ50" s="64"/>
-      <c r="AK50" s="65"/>
-      <c r="AL50" s="64"/>
-      <c r="AM50" s="64"/>
-      <c r="AN50" s="64"/>
-      <c r="AO50" s="64"/>
-      <c r="AP50" s="64"/>
-      <c r="AQ50" s="64"/>
-      <c r="AR50" s="63"/>
-      <c r="AS50" s="64"/>
-      <c r="AT50" s="64"/>
-      <c r="AU50" s="64"/>
-      <c r="AV50" s="64"/>
-      <c r="AW50" s="65"/>
-      <c r="AX50" s="63"/>
-      <c r="AY50" s="64"/>
-      <c r="AZ50" s="64"/>
-      <c r="BA50" s="64"/>
-      <c r="BB50" s="64"/>
-      <c r="BC50" s="65"/>
+      <c r="B50" s="88"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="89"/>
+      <c r="J50" s="89"/>
+      <c r="K50" s="89"/>
+      <c r="L50" s="89"/>
+      <c r="M50" s="90"/>
+      <c r="N50" s="89"/>
+      <c r="O50" s="89"/>
+      <c r="P50" s="89"/>
+      <c r="Q50" s="89"/>
+      <c r="R50" s="89"/>
+      <c r="S50" s="89"/>
+      <c r="T50" s="88"/>
+      <c r="U50" s="89"/>
+      <c r="V50" s="89"/>
+      <c r="W50" s="89"/>
+      <c r="X50" s="89"/>
+      <c r="Y50" s="90"/>
+      <c r="Z50" s="89"/>
+      <c r="AA50" s="89"/>
+      <c r="AB50" s="89"/>
+      <c r="AC50" s="89"/>
+      <c r="AD50" s="89"/>
+      <c r="AE50" s="89"/>
+      <c r="AF50" s="88"/>
+      <c r="AG50" s="89"/>
+      <c r="AH50" s="89"/>
+      <c r="AI50" s="89"/>
+      <c r="AJ50" s="89"/>
+      <c r="AK50" s="90"/>
+      <c r="AL50" s="89"/>
+      <c r="AM50" s="89"/>
+      <c r="AN50" s="89"/>
+      <c r="AO50" s="89"/>
+      <c r="AP50" s="89"/>
+      <c r="AQ50" s="89"/>
+      <c r="AR50" s="88"/>
+      <c r="AS50" s="89"/>
+      <c r="AT50" s="89"/>
+      <c r="AU50" s="89"/>
+      <c r="AV50" s="89"/>
+      <c r="AW50" s="90"/>
+      <c r="AX50" s="88"/>
+      <c r="AY50" s="89"/>
+      <c r="AZ50" s="89"/>
+      <c r="BA50" s="89"/>
+      <c r="BB50" s="89"/>
+      <c r="BC50" s="90"/>
     </row>
     <row r="51" spans="2:55">
-      <c r="B51" s="63"/>
-      <c r="C51" s="64"/>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="65"/>
-      <c r="H51" s="63"/>
-      <c r="I51" s="64"/>
-      <c r="J51" s="64"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="64"/>
-      <c r="M51" s="65"/>
-      <c r="N51" s="64"/>
-      <c r="O51" s="64"/>
-      <c r="P51" s="64"/>
-      <c r="Q51" s="64"/>
-      <c r="R51" s="64"/>
-      <c r="S51" s="64"/>
-      <c r="T51" s="63"/>
-      <c r="U51" s="64"/>
-      <c r="V51" s="64"/>
-      <c r="W51" s="64"/>
-      <c r="X51" s="64"/>
-      <c r="Y51" s="65"/>
-      <c r="Z51" s="64"/>
-      <c r="AA51" s="64"/>
-      <c r="AB51" s="64"/>
-      <c r="AC51" s="64"/>
-      <c r="AD51" s="64"/>
-      <c r="AE51" s="64"/>
-      <c r="AF51" s="63"/>
-      <c r="AG51" s="64"/>
-      <c r="AH51" s="64"/>
-      <c r="AI51" s="64"/>
-      <c r="AJ51" s="64"/>
-      <c r="AK51" s="65"/>
-      <c r="AL51" s="64"/>
-      <c r="AM51" s="64"/>
-      <c r="AN51" s="64"/>
-      <c r="AO51" s="64"/>
-      <c r="AP51" s="64"/>
-      <c r="AQ51" s="64"/>
-      <c r="AR51" s="63"/>
-      <c r="AS51" s="64"/>
-      <c r="AT51" s="64"/>
-      <c r="AU51" s="64"/>
-      <c r="AV51" s="64"/>
-      <c r="AW51" s="65"/>
-      <c r="AX51" s="63"/>
-      <c r="AY51" s="64"/>
-      <c r="AZ51" s="64"/>
-      <c r="BA51" s="64"/>
-      <c r="BB51" s="64"/>
-      <c r="BC51" s="65"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
+      <c r="E51" s="89"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="90"/>
+      <c r="H51" s="88"/>
+      <c r="I51" s="89"/>
+      <c r="J51" s="89"/>
+      <c r="K51" s="89"/>
+      <c r="L51" s="89"/>
+      <c r="M51" s="90"/>
+      <c r="N51" s="89"/>
+      <c r="O51" s="89"/>
+      <c r="P51" s="89"/>
+      <c r="Q51" s="89"/>
+      <c r="R51" s="89"/>
+      <c r="S51" s="89"/>
+      <c r="T51" s="88"/>
+      <c r="U51" s="89"/>
+      <c r="V51" s="89"/>
+      <c r="W51" s="89"/>
+      <c r="X51" s="89"/>
+      <c r="Y51" s="90"/>
+      <c r="Z51" s="89"/>
+      <c r="AA51" s="89"/>
+      <c r="AB51" s="89"/>
+      <c r="AC51" s="89"/>
+      <c r="AD51" s="89"/>
+      <c r="AE51" s="89"/>
+      <c r="AF51" s="88"/>
+      <c r="AG51" s="89"/>
+      <c r="AH51" s="89"/>
+      <c r="AI51" s="89"/>
+      <c r="AJ51" s="89"/>
+      <c r="AK51" s="90"/>
+      <c r="AL51" s="89"/>
+      <c r="AM51" s="89"/>
+      <c r="AN51" s="89"/>
+      <c r="AO51" s="89"/>
+      <c r="AP51" s="89"/>
+      <c r="AQ51" s="89"/>
+      <c r="AR51" s="88"/>
+      <c r="AS51" s="89"/>
+      <c r="AT51" s="89"/>
+      <c r="AU51" s="89"/>
+      <c r="AV51" s="89"/>
+      <c r="AW51" s="90"/>
+      <c r="AX51" s="88"/>
+      <c r="AY51" s="89"/>
+      <c r="AZ51" s="89"/>
+      <c r="BA51" s="89"/>
+      <c r="BB51" s="89"/>
+      <c r="BC51" s="90"/>
     </row>
     <row r="52" spans="2:55">
-      <c r="B52" s="63"/>
-      <c r="C52" s="64"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="63"/>
-      <c r="I52" s="64"/>
-      <c r="J52" s="64"/>
-      <c r="K52" s="64"/>
-      <c r="L52" s="64"/>
-      <c r="M52" s="65"/>
-      <c r="N52" s="64"/>
-      <c r="O52" s="64"/>
-      <c r="P52" s="64"/>
-      <c r="Q52" s="64"/>
-      <c r="R52" s="64"/>
-      <c r="S52" s="64"/>
-      <c r="T52" s="63"/>
-      <c r="U52" s="64"/>
-      <c r="V52" s="64"/>
-      <c r="W52" s="64"/>
-      <c r="X52" s="64"/>
-      <c r="Y52" s="65"/>
-      <c r="Z52" s="64"/>
-      <c r="AA52" s="64"/>
-      <c r="AB52" s="64"/>
-      <c r="AC52" s="64"/>
-      <c r="AD52" s="64"/>
-      <c r="AE52" s="64"/>
-      <c r="AF52" s="63"/>
-      <c r="AG52" s="64"/>
-      <c r="AH52" s="64"/>
-      <c r="AI52" s="64"/>
-      <c r="AJ52" s="64"/>
-      <c r="AK52" s="65"/>
-      <c r="AL52" s="64"/>
-      <c r="AM52" s="64"/>
-      <c r="AN52" s="64"/>
-      <c r="AO52" s="64"/>
-      <c r="AP52" s="64"/>
-      <c r="AQ52" s="64"/>
-      <c r="AR52" s="63"/>
-      <c r="AS52" s="64"/>
-      <c r="AT52" s="64"/>
-      <c r="AU52" s="64"/>
-      <c r="AV52" s="64"/>
-      <c r="AW52" s="65"/>
-      <c r="AX52" s="63"/>
-      <c r="AY52" s="64"/>
-      <c r="AZ52" s="64"/>
-      <c r="BA52" s="64"/>
-      <c r="BB52" s="64"/>
-      <c r="BC52" s="65"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="89"/>
+      <c r="E52" s="89"/>
+      <c r="F52" s="89"/>
+      <c r="G52" s="90"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="89"/>
+      <c r="J52" s="89"/>
+      <c r="K52" s="89"/>
+      <c r="L52" s="89"/>
+      <c r="M52" s="90"/>
+      <c r="N52" s="89"/>
+      <c r="O52" s="89"/>
+      <c r="P52" s="89"/>
+      <c r="Q52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="89"/>
+      <c r="T52" s="88"/>
+      <c r="U52" s="89"/>
+      <c r="V52" s="89"/>
+      <c r="W52" s="89"/>
+      <c r="X52" s="89"/>
+      <c r="Y52" s="90"/>
+      <c r="Z52" s="89"/>
+      <c r="AA52" s="89"/>
+      <c r="AB52" s="89"/>
+      <c r="AC52" s="89"/>
+      <c r="AD52" s="89"/>
+      <c r="AE52" s="89"/>
+      <c r="AF52" s="88"/>
+      <c r="AG52" s="89"/>
+      <c r="AH52" s="89"/>
+      <c r="AI52" s="89"/>
+      <c r="AJ52" s="89"/>
+      <c r="AK52" s="90"/>
+      <c r="AL52" s="89"/>
+      <c r="AM52" s="89"/>
+      <c r="AN52" s="89"/>
+      <c r="AO52" s="89"/>
+      <c r="AP52" s="89"/>
+      <c r="AQ52" s="89"/>
+      <c r="AR52" s="88"/>
+      <c r="AS52" s="89"/>
+      <c r="AT52" s="89"/>
+      <c r="AU52" s="89"/>
+      <c r="AV52" s="89"/>
+      <c r="AW52" s="90"/>
+      <c r="AX52" s="88"/>
+      <c r="AY52" s="89"/>
+      <c r="AZ52" s="89"/>
+      <c r="BA52" s="89"/>
+      <c r="BB52" s="89"/>
+      <c r="BC52" s="90"/>
     </row>
     <row r="53" spans="2:55">
-      <c r="B53" s="63"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="65"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="64"/>
-      <c r="J53" s="64"/>
-      <c r="K53" s="64"/>
-      <c r="L53" s="64"/>
-      <c r="M53" s="65"/>
-      <c r="N53" s="64"/>
-      <c r="O53" s="64"/>
-      <c r="P53" s="64"/>
-      <c r="Q53" s="64"/>
-      <c r="R53" s="64"/>
-      <c r="S53" s="64"/>
-      <c r="T53" s="63"/>
-      <c r="U53" s="64"/>
-      <c r="V53" s="64"/>
-      <c r="W53" s="64"/>
-      <c r="X53" s="64"/>
-      <c r="Y53" s="65"/>
-      <c r="Z53" s="64"/>
-      <c r="AA53" s="64"/>
-      <c r="AB53" s="64"/>
-      <c r="AC53" s="64"/>
-      <c r="AD53" s="64"/>
-      <c r="AE53" s="64"/>
-      <c r="AF53" s="63"/>
-      <c r="AG53" s="64"/>
-      <c r="AH53" s="64"/>
-      <c r="AI53" s="64"/>
-      <c r="AJ53" s="64"/>
-      <c r="AK53" s="65"/>
-      <c r="AL53" s="64"/>
-      <c r="AM53" s="64"/>
-      <c r="AN53" s="64"/>
-      <c r="AO53" s="64"/>
-      <c r="AP53" s="64"/>
-      <c r="AQ53" s="64"/>
-      <c r="AR53" s="63"/>
-      <c r="AS53" s="64"/>
-      <c r="AT53" s="64"/>
-      <c r="AU53" s="64"/>
-      <c r="AV53" s="64"/>
-      <c r="AW53" s="65"/>
-      <c r="AX53" s="63"/>
-      <c r="AY53" s="64"/>
-      <c r="AZ53" s="64"/>
-      <c r="BA53" s="64"/>
-      <c r="BB53" s="64"/>
-      <c r="BC53" s="65"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="90"/>
+      <c r="H53" s="88"/>
+      <c r="I53" s="89"/>
+      <c r="J53" s="89"/>
+      <c r="K53" s="89"/>
+      <c r="L53" s="89"/>
+      <c r="M53" s="90"/>
+      <c r="N53" s="89"/>
+      <c r="O53" s="89"/>
+      <c r="P53" s="89"/>
+      <c r="Q53" s="89"/>
+      <c r="R53" s="89"/>
+      <c r="S53" s="89"/>
+      <c r="T53" s="88"/>
+      <c r="U53" s="89"/>
+      <c r="V53" s="89"/>
+      <c r="W53" s="89"/>
+      <c r="X53" s="89"/>
+      <c r="Y53" s="90"/>
+      <c r="Z53" s="89"/>
+      <c r="AA53" s="89"/>
+      <c r="AB53" s="89"/>
+      <c r="AC53" s="89"/>
+      <c r="AD53" s="89"/>
+      <c r="AE53" s="89"/>
+      <c r="AF53" s="88"/>
+      <c r="AG53" s="89"/>
+      <c r="AH53" s="89"/>
+      <c r="AI53" s="89"/>
+      <c r="AJ53" s="89"/>
+      <c r="AK53" s="90"/>
+      <c r="AL53" s="89"/>
+      <c r="AM53" s="89"/>
+      <c r="AN53" s="89"/>
+      <c r="AO53" s="89"/>
+      <c r="AP53" s="89"/>
+      <c r="AQ53" s="89"/>
+      <c r="AR53" s="88"/>
+      <c r="AS53" s="89"/>
+      <c r="AT53" s="89"/>
+      <c r="AU53" s="89"/>
+      <c r="AV53" s="89"/>
+      <c r="AW53" s="90"/>
+      <c r="AX53" s="88"/>
+      <c r="AY53" s="89"/>
+      <c r="AZ53" s="89"/>
+      <c r="BA53" s="89"/>
+      <c r="BB53" s="89"/>
+      <c r="BC53" s="90"/>
     </row>
     <row r="54" spans="2:55">
-      <c r="B54" s="63"/>
-      <c r="C54" s="64"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="65"/>
-      <c r="H54" s="63"/>
-      <c r="I54" s="64"/>
-      <c r="J54" s="64"/>
-      <c r="K54" s="64"/>
-      <c r="L54" s="64"/>
-      <c r="M54" s="65"/>
-      <c r="N54" s="64"/>
-      <c r="O54" s="64"/>
-      <c r="P54" s="64"/>
-      <c r="Q54" s="64"/>
-      <c r="R54" s="64"/>
-      <c r="S54" s="64"/>
-      <c r="T54" s="63"/>
-      <c r="U54" s="64"/>
-      <c r="V54" s="64"/>
-      <c r="W54" s="64"/>
-      <c r="X54" s="64"/>
-      <c r="Y54" s="65"/>
-      <c r="Z54" s="64"/>
-      <c r="AA54" s="64"/>
-      <c r="AB54" s="64"/>
-      <c r="AC54" s="64"/>
-      <c r="AD54" s="64"/>
-      <c r="AE54" s="64"/>
-      <c r="AF54" s="63"/>
-      <c r="AG54" s="64"/>
-      <c r="AH54" s="64"/>
-      <c r="AI54" s="64"/>
-      <c r="AJ54" s="64"/>
-      <c r="AK54" s="65"/>
-      <c r="AL54" s="64"/>
-      <c r="AM54" s="64"/>
-      <c r="AN54" s="64"/>
-      <c r="AO54" s="64"/>
-      <c r="AP54" s="64"/>
-      <c r="AQ54" s="64"/>
-      <c r="AR54" s="63"/>
-      <c r="AS54" s="64"/>
-      <c r="AT54" s="64"/>
-      <c r="AU54" s="64"/>
-      <c r="AV54" s="64"/>
-      <c r="AW54" s="65"/>
-      <c r="AX54" s="63"/>
-      <c r="AY54" s="64"/>
-      <c r="AZ54" s="64"/>
-      <c r="BA54" s="64"/>
-      <c r="BB54" s="64"/>
-      <c r="BC54" s="65"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="89"/>
+      <c r="E54" s="89"/>
+      <c r="F54" s="89"/>
+      <c r="G54" s="90"/>
+      <c r="H54" s="88"/>
+      <c r="I54" s="89"/>
+      <c r="J54" s="89"/>
+      <c r="K54" s="89"/>
+      <c r="L54" s="89"/>
+      <c r="M54" s="90"/>
+      <c r="N54" s="89"/>
+      <c r="O54" s="89"/>
+      <c r="P54" s="89"/>
+      <c r="Q54" s="89"/>
+      <c r="R54" s="89"/>
+      <c r="S54" s="89"/>
+      <c r="T54" s="88"/>
+      <c r="U54" s="89"/>
+      <c r="V54" s="89"/>
+      <c r="W54" s="89"/>
+      <c r="X54" s="89"/>
+      <c r="Y54" s="90"/>
+      <c r="Z54" s="89"/>
+      <c r="AA54" s="89"/>
+      <c r="AB54" s="89"/>
+      <c r="AC54" s="89"/>
+      <c r="AD54" s="89"/>
+      <c r="AE54" s="89"/>
+      <c r="AF54" s="88"/>
+      <c r="AG54" s="89"/>
+      <c r="AH54" s="89"/>
+      <c r="AI54" s="89"/>
+      <c r="AJ54" s="89"/>
+      <c r="AK54" s="90"/>
+      <c r="AL54" s="89"/>
+      <c r="AM54" s="89"/>
+      <c r="AN54" s="89"/>
+      <c r="AO54" s="89"/>
+      <c r="AP54" s="89"/>
+      <c r="AQ54" s="89"/>
+      <c r="AR54" s="88"/>
+      <c r="AS54" s="89"/>
+      <c r="AT54" s="89"/>
+      <c r="AU54" s="89"/>
+      <c r="AV54" s="89"/>
+      <c r="AW54" s="90"/>
+      <c r="AX54" s="88"/>
+      <c r="AY54" s="89"/>
+      <c r="AZ54" s="89"/>
+      <c r="BA54" s="89"/>
+      <c r="BB54" s="89"/>
+      <c r="BC54" s="90"/>
     </row>
     <row r="55" spans="2:55" ht="15.75" thickBot="1">
-      <c r="B55" s="66"/>
-      <c r="C55" s="67"/>
-      <c r="D55" s="67"/>
-      <c r="E55" s="67"/>
-      <c r="F55" s="67"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="66"/>
-      <c r="I55" s="67"/>
-      <c r="J55" s="67"/>
-      <c r="K55" s="67"/>
-      <c r="L55" s="67"/>
-      <c r="M55" s="68"/>
-      <c r="N55" s="67"/>
-      <c r="O55" s="67"/>
-      <c r="P55" s="67"/>
-      <c r="Q55" s="67"/>
-      <c r="R55" s="67"/>
-      <c r="S55" s="67"/>
-      <c r="T55" s="66"/>
-      <c r="U55" s="67"/>
-      <c r="V55" s="67"/>
-      <c r="W55" s="67"/>
-      <c r="X55" s="67"/>
-      <c r="Y55" s="68"/>
-      <c r="Z55" s="67"/>
-      <c r="AA55" s="67"/>
-      <c r="AB55" s="67"/>
-      <c r="AC55" s="67"/>
-      <c r="AD55" s="67"/>
-      <c r="AE55" s="67"/>
-      <c r="AF55" s="66"/>
-      <c r="AG55" s="67"/>
-      <c r="AH55" s="67"/>
-      <c r="AI55" s="67"/>
-      <c r="AJ55" s="67"/>
-      <c r="AK55" s="68"/>
-      <c r="AL55" s="67"/>
-      <c r="AM55" s="67"/>
-      <c r="AN55" s="67"/>
-      <c r="AO55" s="67"/>
-      <c r="AP55" s="67"/>
-      <c r="AQ55" s="67"/>
-      <c r="AR55" s="66"/>
-      <c r="AS55" s="67"/>
-      <c r="AT55" s="67"/>
-      <c r="AU55" s="67"/>
-      <c r="AV55" s="67"/>
-      <c r="AW55" s="68"/>
-      <c r="AX55" s="66"/>
-      <c r="AY55" s="67"/>
-      <c r="AZ55" s="67"/>
-      <c r="BA55" s="67"/>
-      <c r="BB55" s="67"/>
-      <c r="BC55" s="68"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="92"/>
+      <c r="E55" s="92"/>
+      <c r="F55" s="92"/>
+      <c r="G55" s="93"/>
+      <c r="H55" s="91"/>
+      <c r="I55" s="92"/>
+      <c r="J55" s="92"/>
+      <c r="K55" s="92"/>
+      <c r="L55" s="92"/>
+      <c r="M55" s="93"/>
+      <c r="N55" s="92"/>
+      <c r="O55" s="92"/>
+      <c r="P55" s="92"/>
+      <c r="Q55" s="92"/>
+      <c r="R55" s="92"/>
+      <c r="S55" s="92"/>
+      <c r="T55" s="91"/>
+      <c r="U55" s="92"/>
+      <c r="V55" s="92"/>
+      <c r="W55" s="92"/>
+      <c r="X55" s="92"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="92"/>
+      <c r="AA55" s="92"/>
+      <c r="AB55" s="92"/>
+      <c r="AC55" s="92"/>
+      <c r="AD55" s="92"/>
+      <c r="AE55" s="92"/>
+      <c r="AF55" s="91"/>
+      <c r="AG55" s="92"/>
+      <c r="AH55" s="92"/>
+      <c r="AI55" s="92"/>
+      <c r="AJ55" s="92"/>
+      <c r="AK55" s="93"/>
+      <c r="AL55" s="92"/>
+      <c r="AM55" s="92"/>
+      <c r="AN55" s="92"/>
+      <c r="AO55" s="92"/>
+      <c r="AP55" s="92"/>
+      <c r="AQ55" s="92"/>
+      <c r="AR55" s="91"/>
+      <c r="AS55" s="92"/>
+      <c r="AT55" s="92"/>
+      <c r="AU55" s="92"/>
+      <c r="AV55" s="92"/>
+      <c r="AW55" s="93"/>
+      <c r="AX55" s="91"/>
+      <c r="AY55" s="92"/>
+      <c r="AZ55" s="92"/>
+      <c r="BA55" s="92"/>
+      <c r="BB55" s="92"/>
+      <c r="BC55" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="135">
+    <mergeCell ref="B49:G55"/>
+    <mergeCell ref="B1:AK1"/>
+    <mergeCell ref="AL1:BC1"/>
+    <mergeCell ref="Z4:AE4"/>
+    <mergeCell ref="AF4:AK4"/>
+    <mergeCell ref="AL2:AQ2"/>
+    <mergeCell ref="AL8:AQ8"/>
+    <mergeCell ref="AR2:AW2"/>
+    <mergeCell ref="AR8:AW8"/>
+    <mergeCell ref="AL4:AQ4"/>
+    <mergeCell ref="AR4:AW4"/>
+    <mergeCell ref="Z2:AE2"/>
+    <mergeCell ref="Z8:AE8"/>
+    <mergeCell ref="AF2:AK2"/>
+    <mergeCell ref="AF8:AK8"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="N8:S8"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="T8:Y8"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="AX4:BC4"/>
+    <mergeCell ref="AX19:BB19"/>
+    <mergeCell ref="AX22:BB22"/>
+    <mergeCell ref="AX23:BC27"/>
+    <mergeCell ref="AX28:BC28"/>
+    <mergeCell ref="AZ3:BC3"/>
+    <mergeCell ref="B16:BC16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="AX8:BC8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="T5:Y5"/>
+    <mergeCell ref="Z5:AE5"/>
+    <mergeCell ref="AF5:AK5"/>
+    <mergeCell ref="AL5:AQ5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="AX5:BC5"/>
+    <mergeCell ref="B9:F15"/>
+    <mergeCell ref="H9:M15"/>
+    <mergeCell ref="N9:S15"/>
+    <mergeCell ref="T9:Y15"/>
+    <mergeCell ref="Z9:AE15"/>
+    <mergeCell ref="AF9:AK15"/>
+    <mergeCell ref="AL9:AQ15"/>
+    <mergeCell ref="AZ17:BB17"/>
+    <mergeCell ref="AX18:BB18"/>
+    <mergeCell ref="AR9:AW15"/>
+    <mergeCell ref="AX9:BC15"/>
+    <mergeCell ref="AX44:BC44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="H45:M45"/>
+    <mergeCell ref="N45:S45"/>
+    <mergeCell ref="T45:Y45"/>
+    <mergeCell ref="Z45:AE45"/>
+    <mergeCell ref="AF45:AK45"/>
+    <mergeCell ref="AL45:AQ45"/>
+    <mergeCell ref="AR45:AW45"/>
+    <mergeCell ref="AX45:BC45"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="H44:M44"/>
+    <mergeCell ref="N44:S44"/>
+    <mergeCell ref="T44:Y44"/>
+    <mergeCell ref="Z44:AE44"/>
+    <mergeCell ref="AF44:AK44"/>
+    <mergeCell ref="AL44:AQ44"/>
+    <mergeCell ref="AR44:AW44"/>
+    <mergeCell ref="AR49:AW55"/>
+    <mergeCell ref="AX49:BC55"/>
+    <mergeCell ref="B40:BC40"/>
+    <mergeCell ref="AX39:BC39"/>
+    <mergeCell ref="AX38:BC38"/>
+    <mergeCell ref="AX37:BC37"/>
+    <mergeCell ref="AX36:BC36"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="AL48:AQ48"/>
+    <mergeCell ref="AR48:AW48"/>
+    <mergeCell ref="AX48:BC48"/>
+    <mergeCell ref="H49:M55"/>
+    <mergeCell ref="N49:S55"/>
+    <mergeCell ref="T49:Y55"/>
+    <mergeCell ref="Z49:AE55"/>
+    <mergeCell ref="AF49:AK55"/>
+    <mergeCell ref="AL49:AQ55"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="N48:S48"/>
+    <mergeCell ref="T48:Y48"/>
+    <mergeCell ref="Z48:AE48"/>
+    <mergeCell ref="AF48:AK48"/>
+    <mergeCell ref="BE2:BF2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="AT3:AW3"/>
+    <mergeCell ref="AX2:BC2"/>
     <mergeCell ref="AZ43:BC43"/>
     <mergeCell ref="K23:O23"/>
     <mergeCell ref="D29:F29"/>
@@ -43857,117 +43971,6 @@
     <mergeCell ref="T42:Y42"/>
     <mergeCell ref="Z42:AE42"/>
     <mergeCell ref="AF42:AK42"/>
-    <mergeCell ref="BE2:BF2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="AB3:AE3"/>
-    <mergeCell ref="AH3:AK3"/>
-    <mergeCell ref="AN3:AQ3"/>
-    <mergeCell ref="AT3:AW3"/>
-    <mergeCell ref="AX2:BC2"/>
-    <mergeCell ref="AR49:AW55"/>
-    <mergeCell ref="AX49:BC55"/>
-    <mergeCell ref="B40:BC40"/>
-    <mergeCell ref="AX39:BC39"/>
-    <mergeCell ref="AX38:BC38"/>
-    <mergeCell ref="AX37:BC37"/>
-    <mergeCell ref="AX36:BC36"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="AL48:AQ48"/>
-    <mergeCell ref="AR48:AW48"/>
-    <mergeCell ref="AX48:BC48"/>
-    <mergeCell ref="H49:M55"/>
-    <mergeCell ref="N49:S55"/>
-    <mergeCell ref="T49:Y55"/>
-    <mergeCell ref="Z49:AE55"/>
-    <mergeCell ref="AF49:AK55"/>
-    <mergeCell ref="AL49:AQ55"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="N48:S48"/>
-    <mergeCell ref="T48:Y48"/>
-    <mergeCell ref="Z48:AE48"/>
-    <mergeCell ref="AF48:AK48"/>
-    <mergeCell ref="AX44:BC44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="H45:M45"/>
-    <mergeCell ref="N45:S45"/>
-    <mergeCell ref="T45:Y45"/>
-    <mergeCell ref="Z45:AE45"/>
-    <mergeCell ref="AF45:AK45"/>
-    <mergeCell ref="AL45:AQ45"/>
-    <mergeCell ref="AR45:AW45"/>
-    <mergeCell ref="AX45:BC45"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="H44:M44"/>
-    <mergeCell ref="N44:S44"/>
-    <mergeCell ref="T44:Y44"/>
-    <mergeCell ref="Z44:AE44"/>
-    <mergeCell ref="AF44:AK44"/>
-    <mergeCell ref="AL44:AQ44"/>
-    <mergeCell ref="AR44:AW44"/>
-    <mergeCell ref="B9:F15"/>
-    <mergeCell ref="H9:M15"/>
-    <mergeCell ref="N9:S15"/>
-    <mergeCell ref="T9:Y15"/>
-    <mergeCell ref="Z9:AE15"/>
-    <mergeCell ref="AF9:AK15"/>
-    <mergeCell ref="AL9:AQ15"/>
-    <mergeCell ref="AZ17:BB17"/>
-    <mergeCell ref="AX18:BB18"/>
-    <mergeCell ref="AR9:AW15"/>
-    <mergeCell ref="AX9:BC15"/>
-    <mergeCell ref="AX19:BB19"/>
-    <mergeCell ref="AX22:BB22"/>
-    <mergeCell ref="AX23:BC27"/>
-    <mergeCell ref="AX28:BC28"/>
-    <mergeCell ref="AZ3:BC3"/>
-    <mergeCell ref="B16:BC16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="N4:S4"/>
-    <mergeCell ref="T4:Y4"/>
-    <mergeCell ref="AX8:BC8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="N5:S5"/>
-    <mergeCell ref="T5:Y5"/>
-    <mergeCell ref="Z5:AE5"/>
-    <mergeCell ref="AF5:AK5"/>
-    <mergeCell ref="AL5:AQ5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="AX5:BC5"/>
-    <mergeCell ref="B49:G55"/>
-    <mergeCell ref="B1:AK1"/>
-    <mergeCell ref="AL1:BC1"/>
-    <mergeCell ref="Z4:AE4"/>
-    <mergeCell ref="AF4:AK4"/>
-    <mergeCell ref="AL2:AQ2"/>
-    <mergeCell ref="AL8:AQ8"/>
-    <mergeCell ref="AR2:AW2"/>
-    <mergeCell ref="AR8:AW8"/>
-    <mergeCell ref="AL4:AQ4"/>
-    <mergeCell ref="AR4:AW4"/>
-    <mergeCell ref="Z2:AE2"/>
-    <mergeCell ref="Z8:AE8"/>
-    <mergeCell ref="AF2:AK2"/>
-    <mergeCell ref="AF8:AK8"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="N8:S8"/>
-    <mergeCell ref="T2:Y2"/>
-    <mergeCell ref="T8:Y8"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="AX4:BC4"/>
   </mergeCells>
   <conditionalFormatting sqref="BG3 BG10">
     <cfRule type="notContainsText" dxfId="1" priority="2" operator="notContains" text="CREW">
@@ -49491,7 +49494,7 @@
       </c>
       <c r="AF9" s="2" t="str">
         <f>INDEX(TblCardDesign[#Data],MATCH($R9,TblCardDesign[ID],0),17)</f>
-        <v>Add the start of your Resource Allocation Phase, increment your Handling dice by 1</v>
+        <v>At the start of your Resource Allocation Phase, increment your Handling dice by 1</v>
       </c>
       <c r="AI9">
         <v>149</v>

</xml_diff>